<commit_message>
Correction de format de date #3
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele.xlsx
+++ b/fichiers/conf/modele.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sébastien\Dropbox\Seb\SGDF\outilssgdf\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E9E044-6182-4A08-86CA-323F11DC8923}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8A9A17-EC63-4676-966C-2951C8E7840F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3360" yWindow="0" windowWidth="28800" windowHeight="11625" tabRatio="458" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
@@ -1327,7 +1327,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1512,6 +1512,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2315,17 +2333,15 @@
     <col min="6" max="6" width="13.28515625" style="28" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" style="2" customWidth="1"/>
     <col min="8" max="8" width="2.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="28" customWidth="1"/>
-    <col min="11" max="12" width="11.42578125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="28" customWidth="1"/>
-    <col min="14" max="14" width="17.7109375" style="28" customWidth="1"/>
+    <col min="9" max="12" width="11.42578125" style="71" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="75" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" style="75" customWidth="1"/>
     <col min="15" max="15" width="2.5703125" style="28" customWidth="1"/>
     <col min="16" max="16" width="14.7109375" style="28" customWidth="1"/>
     <col min="17" max="17" width="2.85546875" style="2" customWidth="1"/>
-    <col min="18" max="22" width="11.42578125" style="2" customWidth="1"/>
+    <col min="18" max="22" width="11.42578125" style="71" customWidth="1"/>
     <col min="23" max="23" width="3.140625" style="2" customWidth="1"/>
-    <col min="24" max="30" width="11.42578125" style="2" customWidth="1"/>
+    <col min="24" max="30" width="11.42578125" style="71" customWidth="1"/>
     <col min="31" max="31" width="11.42578125" style="28" customWidth="1"/>
     <col min="32" max="32" width="12.7109375" style="2" customWidth="1"/>
     <col min="33" max="33" width="15" style="28" customWidth="1"/>
@@ -2357,22 +2373,22 @@
       <c r="H1" s="64" t="s">
         <v>121</v>
       </c>
-      <c r="I1" s="59" t="s">
+      <c r="I1" s="70" t="s">
         <v>122</v>
       </c>
-      <c r="J1" s="59" t="s">
+      <c r="J1" s="70" t="s">
         <v>123</v>
       </c>
-      <c r="K1" s="59" t="s">
+      <c r="K1" s="70" t="s">
         <v>124</v>
       </c>
-      <c r="L1" s="59" t="s">
+      <c r="L1" s="70" t="s">
         <v>125</v>
       </c>
-      <c r="M1" s="59" t="s">
+      <c r="M1" s="74" t="s">
         <v>138</v>
       </c>
-      <c r="N1" s="59" t="s">
+      <c r="N1" s="74" t="s">
         <v>139</v>
       </c>
       <c r="O1" s="64" t="s">
@@ -2384,43 +2400,43 @@
       <c r="Q1" s="64" t="s">
         <v>121</v>
       </c>
-      <c r="R1" s="61" t="s">
+      <c r="R1" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="61" t="s">
+      <c r="S1" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="61" t="s">
+      <c r="T1" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="61" t="s">
+      <c r="U1" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="61" t="s">
+      <c r="V1" s="72" t="s">
         <v>12</v>
       </c>
       <c r="W1" s="64" t="s">
         <v>121</v>
       </c>
-      <c r="X1" s="62" t="s">
+      <c r="X1" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="Y1" s="62" t="s">
+      <c r="Y1" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" s="62" t="s">
+      <c r="Z1" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="AA1" s="62" t="s">
+      <c r="AA1" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="AB1" s="62" t="s">
+      <c r="AB1" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="AC1" s="62" t="s">
+      <c r="AC1" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="AD1" s="62" t="s">
+      <c r="AD1" s="73" t="s">
         <v>17</v>
       </c>
       <c r="AE1" s="64" t="s">
@@ -2458,22 +2474,22 @@
       <c r="G2" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="71" t="s">
         <v>115</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="71" t="s">
         <v>114</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="75" t="s">
         <v>142</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="75" t="s">
         <v>141</v>
       </c>
       <c r="O2" s="10"/>
@@ -2481,41 +2497,41 @@
         <v>107</v>
       </c>
       <c r="Q2" s="10"/>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U2" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V2" s="71" t="s">
         <v>52</v>
       </c>
       <c r="W2" s="10"/>
-      <c r="X2" s="3" t="s">
+      <c r="X2" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Y2" s="71" t="s">
         <v>54</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Z2" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AA2" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AB2" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AC2" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AD2" s="71" t="s">
         <v>140</v>
       </c>
       <c r="AE2" s="3"/>
@@ -2554,22 +2570,22 @@
       <c r="G3" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="71" t="s">
         <v>115</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="71" t="s">
         <v>114</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="75" t="s">
         <v>142</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="75" t="s">
         <v>141</v>
       </c>
       <c r="O3" s="10"/>
@@ -2577,41 +2593,41 @@
         <v>107</v>
       </c>
       <c r="Q3" s="10"/>
-      <c r="R3" s="3" t="s">
+      <c r="R3" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="S3" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="T3" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="U3" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="V3" s="71" t="s">
         <v>52</v>
       </c>
       <c r="W3" s="10"/>
-      <c r="X3" s="3" t="s">
+      <c r="X3" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="Y3" s="71" t="s">
         <v>54</v>
       </c>
-      <c r="Z3" s="3" t="s">
+      <c r="Z3" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="AA3" s="3" t="s">
+      <c r="AA3" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="AB3" s="3" t="s">
+      <c r="AB3" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AC3" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="AD3" s="3" t="s">
+      <c r="AD3" s="71" t="s">
         <v>140</v>
       </c>
       <c r="AE3" s="3"/>
@@ -3250,11 +3266,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="7" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="70"/>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="72"/>
+      <c r="A1" s="76"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="78"/>
       <c r="F1" s="64" t="s">
         <v>121</v>
       </c>
@@ -3273,34 +3289,34 @@
       <c r="K1" s="64" t="s">
         <v>121</v>
       </c>
-      <c r="L1" s="73" t="s">
+      <c r="L1" s="79" t="s">
         <v>64</v>
       </c>
-      <c r="M1" s="74"/>
-      <c r="N1" s="75"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="81"/>
       <c r="O1" s="64" t="s">
         <v>121</v>
       </c>
-      <c r="P1" s="76" t="s">
+      <c r="P1" s="82" t="s">
         <v>65</v>
       </c>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="78"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="84"/>
       <c r="S1" s="64" t="s">
         <v>121</v>
       </c>
-      <c r="T1" s="76" t="s">
+      <c r="T1" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="U1" s="78"/>
+      <c r="U1" s="84"/>
       <c r="V1" s="64" t="s">
         <v>121</v>
       </c>
-      <c r="W1" s="73" t="s">
+      <c r="W1" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="X1" s="74"/>
-      <c r="Y1" s="75"/>
+      <c r="X1" s="80"/>
+      <c r="Y1" s="81"/>
     </row>
     <row r="2" spans="1:26" s="16" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="67" t="s">
@@ -3504,7 +3520,9 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3517,7 +3535,7 @@
         <v>39</v>
       </c>
       <c r="B1" s="68">
-        <v>43432</v>
+        <v>43439</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ajout du bafa/bafd civils
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele.xlsx
+++ b/fichiers/conf/modele.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE50D63-5C9C-41A5-A144-D1F5A99A5DDB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE5EDB4-0D31-4FF5-8D17-6E64CC799444}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="0" windowWidth="28800" windowHeight="11625" tabRatio="466" activeTab="3" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="3360" yWindow="0" windowWidth="28800" windowHeight="11625" tabRatio="466" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Responsables" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Quotas Camps'!$A$2:$E$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Responsables!$A$1:$AI$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Responsables!$A$1:$AM$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Synthèse par unité'!$A$1:$R$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -263,7 +263,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{D7CCADB1-4D8A-4BC8-905C-D1BA438E77F1}">
+    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{D7CCADB1-4D8A-4BC8-905C-D1BA438E77F1}">
       <text>
         <r>
           <rPr>
@@ -287,7 +287,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{E9756D3C-D426-47A5-A95D-19409772C521}">
+    <comment ref="AC1" authorId="0" shapeId="0" xr:uid="{E9756D3C-D426-47A5-A95D-19409772C521}">
       <text>
         <r>
           <rPr>
@@ -311,7 +311,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{2F31B678-BEA5-4DB4-AC1D-AC1EC879D750}">
+    <comment ref="AD1" authorId="0" shapeId="0" xr:uid="{2F31B678-BEA5-4DB4-AC1D-AC1EC879D750}">
       <text>
         <r>
           <rPr>
@@ -335,7 +335,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{C8A48C2F-9EB4-4B10-8DBC-DE0A2B010CD5}">
+    <comment ref="AE1" authorId="0" shapeId="0" xr:uid="{C8A48C2F-9EB4-4B10-8DBC-DE0A2B010CD5}">
       <text>
         <r>
           <rPr>
@@ -359,7 +359,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{CE08BEFE-EAC8-4844-983C-8BADEFBFE2C5}">
+    <comment ref="AF1" authorId="0" shapeId="0" xr:uid="{CE08BEFE-EAC8-4844-983C-8BADEFBFE2C5}">
       <text>
         <r>
           <rPr>
@@ -383,7 +383,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="0" shapeId="0" xr:uid="{28DEFE86-2BEB-4C19-99F9-9FC3C46725F3}">
+    <comment ref="AG1" authorId="0" shapeId="0" xr:uid="{28DEFE86-2BEB-4C19-99F9-9FC3C46725F3}">
       <text>
         <r>
           <rPr>
@@ -407,7 +407,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD1" authorId="0" shapeId="0" xr:uid="{9189F978-0462-4031-826A-0220C3A0FBE8}">
+    <comment ref="AH1" authorId="0" shapeId="0" xr:uid="{9189F978-0462-4031-826A-0220C3A0FBE8}">
       <text>
         <r>
           <rPr>
@@ -431,7 +431,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF1" authorId="0" shapeId="0" xr:uid="{C19C0D7F-4226-4736-BA35-E6E08EBBAC7A}">
+    <comment ref="AJ1" authorId="0" shapeId="0" xr:uid="{C19C0D7F-4226-4736-BA35-E6E08EBBAC7A}">
       <text>
         <r>
           <rPr>
@@ -455,7 +455,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG1" authorId="0" shapeId="0" xr:uid="{AB0FF933-2837-4C7D-A183-D59581906014}">
+    <comment ref="AK1" authorId="0" shapeId="0" xr:uid="{AB0FF933-2837-4C7D-A183-D59581906014}">
       <text>
         <r>
           <rPr>
@@ -479,7 +479,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH1" authorId="0" shapeId="0" xr:uid="{783213B1-12E4-4FD7-BD87-ED5859C4959C}">
+    <comment ref="AL1" authorId="0" shapeId="0" xr:uid="{783213B1-12E4-4FD7-BD87-ED5859C4959C}">
       <text>
         <r>
           <rPr>
@@ -602,7 +602,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="173">
   <si>
     <t>&lt;/jt:forEach&gt;</t>
   </si>
@@ -1110,6 +1110,30 @@
   </si>
   <si>
     <t>$[CEILING($D4*0.8/12,1)]</t>
+  </si>
+  <si>
+    <t>MARI</t>
+  </si>
+  <si>
+    <t>BAFA GENERAL</t>
+  </si>
+  <si>
+    <t>BAFD GENERAL</t>
+  </si>
+  <si>
+    <t>BAFD PERFECTIONNEMENT</t>
+  </si>
+  <si>
+    <t>${chef.formation.mari.datefin}</t>
+  </si>
+  <si>
+    <t>${chef.formation.bafa_general.datefin}</t>
+  </si>
+  <si>
+    <t>${chef.formation.bafd_general.datefin}</t>
+  </si>
+  <si>
+    <t>${chef.formation.bafd_perfectionnement.datefin}</t>
   </si>
 </sst>
 </file>
@@ -1588,6 +1612,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1614,30 +1662,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2214,13 +2238,13 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:AI3"/>
+  <dimension ref="A1:AM3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="AC2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AH2" sqref="AH2"/>
+      <selection pane="bottomRight" activeCell="W1" sqref="W1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2239,16 +2263,17 @@
     <col min="15" max="15" width="2.5703125" style="26" customWidth="1"/>
     <col min="16" max="16" width="14.7109375" style="26" customWidth="1"/>
     <col min="17" max="17" width="2.85546875" style="2" customWidth="1"/>
-    <col min="18" max="22" width="11.42578125" style="49" customWidth="1"/>
-    <col min="23" max="23" width="3.140625" style="2" customWidth="1"/>
-    <col min="24" max="30" width="11.42578125" style="49" customWidth="1"/>
-    <col min="31" max="31" width="11.42578125" style="26" customWidth="1"/>
-    <col min="32" max="32" width="12.7109375" style="2" customWidth="1"/>
-    <col min="33" max="33" width="15" style="26" customWidth="1"/>
-    <col min="34" max="34" width="14.140625" style="26" customWidth="1"/>
+    <col min="18" max="25" width="11.42578125" style="49" customWidth="1"/>
+    <col min="26" max="26" width="17.5703125" style="49" customWidth="1"/>
+    <col min="27" max="27" width="3.140625" style="2" customWidth="1"/>
+    <col min="28" max="34" width="11.42578125" style="49" customWidth="1"/>
+    <col min="35" max="35" width="11.42578125" style="26" customWidth="1"/>
+    <col min="36" max="36" width="12.7109375" style="2" customWidth="1"/>
+    <col min="37" max="37" width="15" style="26" customWidth="1"/>
+    <col min="38" max="38" width="14.140625" style="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="41" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39" s="41" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
         <v>3</v>
       </c>
@@ -2315,44 +2340,56 @@
       <c r="V1" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="W1" s="42" t="s">
+      <c r="W1" s="50" t="s">
+        <v>165</v>
+      </c>
+      <c r="X1" s="50" t="s">
+        <v>166</v>
+      </c>
+      <c r="Y1" s="50" t="s">
+        <v>167</v>
+      </c>
+      <c r="Z1" s="50" t="s">
+        <v>168</v>
+      </c>
+      <c r="AA1" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="X1" s="51" t="s">
+      <c r="AB1" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="Y1" s="51" t="s">
+      <c r="AC1" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" s="51" t="s">
+      <c r="AD1" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="AA1" s="51" t="s">
+      <c r="AE1" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="AB1" s="51" t="s">
+      <c r="AF1" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="AC1" s="51" t="s">
+      <c r="AG1" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="AD1" s="51" t="s">
+      <c r="AH1" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="AE1" s="42" t="s">
+      <c r="AI1" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="AF1" s="33" t="s">
+      <c r="AJ1" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="AG1" s="36" t="s">
+      <c r="AK1" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="AH1" s="36" t="s">
+      <c r="AL1" s="36" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>92</v>
       </c>
@@ -2412,43 +2449,55 @@
       <c r="V2" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="W2" s="10"/>
+      <c r="W2" s="49" t="s">
+        <v>169</v>
+      </c>
       <c r="X2" s="49" t="s">
+        <v>170</v>
+      </c>
+      <c r="Y2" s="49" t="s">
+        <v>171</v>
+      </c>
+      <c r="Z2" s="49" t="s">
+        <v>172</v>
+      </c>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="Y2" s="49" t="s">
+      <c r="AC2" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="Z2" s="49" t="s">
+      <c r="AD2" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="AA2" s="49" t="s">
+      <c r="AE2" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="AB2" s="49" t="s">
+      <c r="AF2" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="AC2" s="49" t="s">
+      <c r="AG2" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="AD2" s="49" t="s">
+      <c r="AH2" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="47" t="s">
+      <c r="AI2" s="3"/>
+      <c r="AJ2" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AK2" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AL2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AM2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:35" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
         <v>96</v>
       </c>
@@ -2508,50 +2557,62 @@
       <c r="V3" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="W3" s="10"/>
+      <c r="W3" s="49" t="s">
+        <v>169</v>
+      </c>
       <c r="X3" s="49" t="s">
+        <v>170</v>
+      </c>
+      <c r="Y3" s="49" t="s">
+        <v>171</v>
+      </c>
+      <c r="Z3" s="49" t="s">
+        <v>172</v>
+      </c>
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="Y3" s="49" t="s">
+      <c r="AC3" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="Z3" s="49" t="s">
+      <c r="AD3" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="AA3" s="49" t="s">
+      <c r="AE3" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="AB3" s="49" t="s">
+      <c r="AF3" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="AC3" s="49" t="s">
+      <c r="AG3" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="AD3" s="49" t="s">
+      <c r="AH3" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="AE3" s="3"/>
-      <c r="AF3" s="47" t="s">
+      <c r="AI3" s="3"/>
+      <c r="AJ3" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="AG3" s="3" t="s">
+      <c r="AK3" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="AH3" s="3" t="s">
+      <c r="AL3" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AI3" s="25" t="s">
+      <c r="AM3" s="25" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AI3" xr:uid="{D6BF73C0-3DFA-4EF7-83FF-A6F179361B6B}"/>
-  <conditionalFormatting sqref="AH2:AH65536">
+  <autoFilter ref="A1:AM3" xr:uid="{D6BF73C0-3DFA-4EF7-83FF-A6F179361B6B}"/>
+  <conditionalFormatting sqref="AL2:AL65536">
     <cfRule type="cellIs" dxfId="24" priority="24" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG2:AG65536">
+  <conditionalFormatting sqref="AK2:AK65536">
     <cfRule type="cellIs" dxfId="23" priority="14" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
@@ -2822,38 +2883,38 @@
       <c r="P1" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="Q1" s="82" t="s">
+      <c r="Q1" s="90" t="s">
         <v>110</v>
       </c>
-      <c r="R1" s="83"/>
-      <c r="S1" s="84"/>
+      <c r="R1" s="91"/>
+      <c r="S1" s="92"/>
       <c r="T1" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="U1" s="82" t="s">
+      <c r="U1" s="90" t="s">
         <v>157</v>
       </c>
-      <c r="V1" s="85"/>
-      <c r="W1" s="86"/>
+      <c r="V1" s="93"/>
+      <c r="W1" s="94"/>
       <c r="X1" s="57"/>
-      <c r="Y1" s="82" t="s">
+      <c r="Y1" s="90" t="s">
         <v>158</v>
       </c>
-      <c r="Z1" s="85"/>
-      <c r="AA1" s="86"/>
-      <c r="AB1" s="82" t="s">
+      <c r="Z1" s="93"/>
+      <c r="AA1" s="94"/>
+      <c r="AB1" s="90" t="s">
         <v>154</v>
       </c>
-      <c r="AC1" s="85"/>
-      <c r="AD1" s="85"/>
+      <c r="AC1" s="93"/>
+      <c r="AD1" s="93"/>
       <c r="AE1" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="AF1" s="87" t="s">
+      <c r="AF1" s="95" t="s">
         <v>44</v>
       </c>
-      <c r="AG1" s="83"/>
-      <c r="AH1" s="84"/>
+      <c r="AG1" s="91"/>
+      <c r="AH1" s="92"/>
     </row>
     <row r="2" spans="1:35" s="54" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="55"/>
@@ -2895,43 +2956,43 @@
       </c>
       <c r="B3" s="65"/>
       <c r="C3" s="65"/>
-      <c r="D3" s="98" t="s">
+      <c r="D3" s="89" t="s">
         <v>111</v>
       </c>
-      <c r="E3" s="98" t="s">
+      <c r="E3" s="89" t="s">
         <v>112</v>
       </c>
-      <c r="F3" s="91" t="s">
+      <c r="F3" s="82" t="s">
         <v>113</v>
       </c>
-      <c r="G3" s="91" t="s">
+      <c r="G3" s="82" t="s">
         <v>114</v>
       </c>
-      <c r="H3" s="91" t="s">
+      <c r="H3" s="82" t="s">
         <v>115</v>
       </c>
-      <c r="I3" s="91" t="s">
+      <c r="I3" s="82" t="s">
         <v>116</v>
       </c>
-      <c r="J3" s="91" t="s">
+      <c r="J3" s="82" t="s">
         <v>117</v>
       </c>
-      <c r="K3" s="92" t="s">
+      <c r="K3" s="83" t="s">
         <v>118</v>
       </c>
-      <c r="L3" s="93" t="s">
+      <c r="L3" s="84" t="s">
         <v>119</v>
       </c>
-      <c r="M3" s="94" t="s">
+      <c r="M3" s="85" t="s">
         <v>120</v>
       </c>
-      <c r="N3" s="94" t="s">
+      <c r="N3" s="85" t="s">
         <v>121</v>
       </c>
-      <c r="O3" s="95" t="s">
+      <c r="O3" s="86" t="s">
         <v>122</v>
       </c>
-      <c r="P3" s="96" t="s">
+      <c r="P3" s="87" t="s">
         <v>123</v>
       </c>
       <c r="Q3" s="19" t="s">
@@ -2943,7 +3004,7 @@
       <c r="S3" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="T3" s="96" t="s">
+      <c r="T3" s="87" t="s">
         <v>124</v>
       </c>
       <c r="U3" s="19" t="s">
@@ -2955,7 +3016,7 @@
       <c r="W3" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="X3" s="97" t="s">
+      <c r="X3" s="88" t="s">
         <v>125</v>
       </c>
       <c r="Y3" s="81" t="s">
@@ -2976,7 +3037,7 @@
       <c r="AD3" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="AE3" s="96" t="s">
+      <c r="AE3" s="87" t="s">
         <v>126</v>
       </c>
       <c r="AF3" s="19" t="s">
@@ -3169,7 +3230,7 @@
   </sheetPr>
   <dimension ref="A1:AL16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -3207,11 +3268,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" s="7" customFormat="1" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="88"/>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="90"/>
+      <c r="A1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="98"/>
       <c r="F1" s="26"/>
       <c r="G1" s="36" t="s">
         <v>106</v>
@@ -3246,39 +3307,39 @@
       <c r="Q1" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="R1" s="87" t="s">
+      <c r="R1" s="95" t="s">
         <v>63</v>
       </c>
-      <c r="S1" s="83"/>
-      <c r="T1" s="84"/>
+      <c r="S1" s="91"/>
+      <c r="T1" s="92"/>
       <c r="U1" s="42"/>
-      <c r="V1" s="82" t="s">
+      <c r="V1" s="90" t="s">
         <v>156</v>
       </c>
-      <c r="W1" s="83"/>
-      <c r="X1" s="84"/>
+      <c r="W1" s="91"/>
+      <c r="X1" s="92"/>
       <c r="Y1" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="Z1" s="82" t="s">
+      <c r="Z1" s="90" t="s">
         <v>155</v>
       </c>
-      <c r="AA1" s="85"/>
-      <c r="AB1" s="86"/>
+      <c r="AA1" s="93"/>
+      <c r="AB1" s="94"/>
       <c r="AC1" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="AD1" s="82" t="s">
+      <c r="AD1" s="90" t="s">
         <v>154</v>
       </c>
-      <c r="AE1" s="85"/>
-      <c r="AF1" s="86"/>
+      <c r="AE1" s="93"/>
+      <c r="AF1" s="94"/>
       <c r="AG1" s="25"/>
-      <c r="AH1" s="87" t="s">
+      <c r="AH1" s="95" t="s">
         <v>44</v>
       </c>
-      <c r="AI1" s="83"/>
-      <c r="AJ1" s="84"/>
+      <c r="AI1" s="91"/>
+      <c r="AJ1" s="92"/>
     </row>
     <row r="2" spans="1:38" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="45" t="s">
@@ -3297,19 +3358,19 @@
         <v>20</v>
       </c>
       <c r="F2" s="26"/>
-      <c r="G2" s="91" t="s">
+      <c r="G2" s="82" t="s">
         <v>113</v>
       </c>
-      <c r="H2" s="91" t="s">
+      <c r="H2" s="82" t="s">
         <v>114</v>
       </c>
-      <c r="I2" s="91" t="s">
+      <c r="I2" s="82" t="s">
         <v>115</v>
       </c>
-      <c r="J2" s="91" t="s">
+      <c r="J2" s="82" t="s">
         <v>116</v>
       </c>
-      <c r="K2" s="91" t="s">
+      <c r="K2" s="82" t="s">
         <v>117</v>
       </c>
       <c r="L2" s="18"/>
@@ -3539,7 +3600,7 @@
         <v>39</v>
       </c>
       <c r="B1" s="46">
-        <v>43439</v>
+        <v>43477</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Calcul des quotas #9
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele.xlsx
+++ b/fichiers/conf/modele.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE5EDB4-0D31-4FF5-8D17-6E64CC799444}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9865C64-73FA-404A-8242-D45AEC6A8E25}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="0" windowWidth="28800" windowHeight="11625" tabRatio="466" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="3360" yWindow="0" windowWidth="28800" windowHeight="11625" tabRatio="466" activeTab="6" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Responsables" sheetId="1" r:id="rId1"/>
@@ -573,7 +573,7 @@
     <author>Sébastien</author>
   </authors>
   <commentList>
-    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{817EB142-B72A-4675-AB9B-D64CBC1329A3}">
+    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{1D548B4D-EF32-4C8F-95A2-E8B4007C39F1}">
       <text>
         <r>
           <rPr>
@@ -602,7 +602,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="181">
   <si>
     <t>&lt;/jt:forEach&gt;</t>
   </si>
@@ -830,9 +830,6 @@
   </si>
   <si>
     <t>${chef.codestructure}</t>
-  </si>
-  <si>
-    <t>Manque</t>
   </si>
   <si>
     <t>${unite.codestructure}</t>
@@ -1044,9 +1041,6 @@
     <t>$[AA3-Z3]</t>
   </si>
   <si>
-    <t>$[AD3-AE3]</t>
-  </si>
-  <si>
     <t>$[T3]</t>
   </si>
   <si>
@@ -1063,9 +1057,6 @@
   </si>
   <si>
     <t>${unite.psc1afps}</t>
-  </si>
-  <si>
-    <t>$[AH3-AI3]</t>
   </si>
   <si>
     <t>Encadrement 2ème étape
@@ -1074,16 +1065,6 @@
 1 dir titulaire</t>
   </si>
   <si>
-    <t>Encadrement 2ème étape
-par rapport au minimum de animateurs : 
-50% titulaire + 1 dir titulaire</t>
-  </si>
-  <si>
-    <t>Encadrement 1ère étape
-1 chef pour 12 jeunes
-plus directeur</t>
-  </si>
-  <si>
     <t>Encadrement 1ère étape
 1 animateur pour 12 jeunes
 plus directeur</t>
@@ -1134,13 +1115,60 @@
   </si>
   <si>
     <t>${chef.formation.bafd_perfectionnement.datefin}</t>
+  </si>
+  <si>
+    <t>Encadrement 1ère étape
+1 chef pour 12 jeunes
+plus directeur
+sauf unité rouge ou verte</t>
+  </si>
+  <si>
+    <t>Encadrement 2ème étape
+par rapport au minimum de animateurs : 
+50% titulaire + 1 dir titulaire (sauf rouge/vert)</t>
+  </si>
+  <si>
+    <t>Encadrement 2ème étape
+par rapport au minimum d'animateurs : 
+80% titulaire ou stagiaire +
+1 dir titulaire (sauf rouge/vert)</t>
+  </si>
+  <si>
+    <t>$[AE3-AD3]</t>
+  </si>
+  <si>
+    <t>$[AI3-AH3]</t>
+  </si>
+  <si>
+    <t>$[E3]</t>
+  </si>
+  <si>
+    <t>${unite.qualifieannee}</t>
+  </si>
+  <si>
+    <t>${unite.toutsf}</t>
+  </si>
+  <si>
+    <t>$[IF($B3=$C3,0,1)]</t>
+  </si>
+  <si>
+    <t>Unite</t>
+  </si>
+  <si>
+    <t>$[CEILING($D3/12,1)+IF(VALUE(C3)-VALUE(B3)&lt;30,1,0)]</t>
+  </si>
+  <si>
+    <t>$[CEILING($D3*0.5/12,1)+IF(VALUE(C3)-VALUE(B3)&lt;30,1,0)]</t>
+  </si>
+  <si>
+    <t>$[CEILING($D3*0.8/12,1)+IF(VALUE(C3)-VALUE(B3)&lt;30,1,0)]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1200,14 +1228,6 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1391,7 +1411,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1462,9 +1482,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1475,43 +1492,43 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1520,19 +1537,19 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1612,30 +1629,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1654,14 +1674,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1669,7 +1704,167 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="139">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -1797,6 +1992,981 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2240,11 +3410,11 @@
   </sheetPr>
   <dimension ref="A1:AM3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W1" sqref="W1:Z1"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2257,141 +3427,141 @@
     <col min="6" max="6" width="13.28515625" style="26" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" style="2" customWidth="1"/>
     <col min="8" max="8" width="2.85546875" customWidth="1"/>
-    <col min="9" max="12" width="11.42578125" style="49" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="53" customWidth="1"/>
-    <col min="14" max="14" width="17.7109375" style="53" customWidth="1"/>
+    <col min="9" max="12" width="11.42578125" style="48" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="52" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" style="52" customWidth="1"/>
     <col min="15" max="15" width="2.5703125" style="26" customWidth="1"/>
     <col min="16" max="16" width="14.7109375" style="26" customWidth="1"/>
     <col min="17" max="17" width="2.85546875" style="2" customWidth="1"/>
-    <col min="18" max="25" width="11.42578125" style="49" customWidth="1"/>
-    <col min="26" max="26" width="17.5703125" style="49" customWidth="1"/>
+    <col min="18" max="25" width="11.42578125" style="48" customWidth="1"/>
+    <col min="26" max="26" width="17.5703125" style="48" customWidth="1"/>
     <col min="27" max="27" width="3.140625" style="2" customWidth="1"/>
-    <col min="28" max="34" width="11.42578125" style="49" customWidth="1"/>
+    <col min="28" max="34" width="11.42578125" style="48" customWidth="1"/>
     <col min="35" max="35" width="11.42578125" style="26" customWidth="1"/>
     <col min="36" max="36" width="12.7109375" style="2" customWidth="1"/>
     <col min="37" max="37" width="15" style="26" customWidth="1"/>
     <col min="38" max="38" width="14.140625" style="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="41" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:39" s="40" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="36" t="s">
-        <v>93</v>
-      </c>
-      <c r="F1" s="36" t="s">
+      <c r="E1" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="H1" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="J1" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="J1" s="48" t="s">
+      <c r="K1" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="48" t="s">
+      <c r="L1" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="L1" s="48" t="s">
-        <v>88</v>
-      </c>
-      <c r="M1" s="52" t="s">
+      <c r="M1" s="51" t="s">
+        <v>99</v>
+      </c>
+      <c r="N1" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="N1" s="52" t="s">
-        <v>101</v>
-      </c>
-      <c r="O1" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="P1" s="38" t="s">
+      <c r="O1" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="P1" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="Q1" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="R1" s="50" t="s">
+      <c r="Q1" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="R1" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="50" t="s">
+      <c r="S1" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="50" t="s">
+      <c r="T1" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="50" t="s">
+      <c r="U1" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="50" t="s">
+      <c r="V1" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="W1" s="50" t="s">
-        <v>165</v>
-      </c>
-      <c r="X1" s="50" t="s">
-        <v>166</v>
-      </c>
-      <c r="Y1" s="50" t="s">
-        <v>167</v>
-      </c>
-      <c r="Z1" s="50" t="s">
-        <v>168</v>
-      </c>
-      <c r="AA1" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="AB1" s="51" t="s">
+      <c r="W1" s="49" t="s">
+        <v>160</v>
+      </c>
+      <c r="X1" s="49" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y1" s="49" t="s">
+        <v>162</v>
+      </c>
+      <c r="Z1" s="49" t="s">
+        <v>163</v>
+      </c>
+      <c r="AA1" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB1" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="AC1" s="51" t="s">
+      <c r="AC1" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" s="51" t="s">
+      <c r="AD1" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="AE1" s="51" t="s">
+      <c r="AE1" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="AF1" s="51" t="s">
+      <c r="AF1" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="AG1" s="51" t="s">
+      <c r="AG1" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="AH1" s="51" t="s">
+      <c r="AH1" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="AI1" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="AJ1" s="33" t="s">
+      <c r="AI1" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ1" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="AK1" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="AL1" s="36" t="s">
-        <v>83</v>
+      <c r="AK1" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="AL1" s="35" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -2403,7 +3573,7 @@
         <v>61</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F2" s="24" t="s">
         <v>75</v>
@@ -2411,84 +3581,84 @@
       <c r="G2" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="I2" s="49" t="s">
-        <v>79</v>
-      </c>
-      <c r="J2" s="49" t="s">
+      <c r="I2" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="K2" s="49" t="s">
+      <c r="J2" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="L2" s="49" t="s">
+      <c r="L2" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="M2" s="53" t="s">
-        <v>104</v>
-      </c>
-      <c r="N2" s="53" t="s">
+      <c r="M2" s="52" t="s">
         <v>103</v>
+      </c>
+      <c r="N2" s="52" t="s">
+        <v>102</v>
       </c>
       <c r="O2" s="10"/>
       <c r="P2" s="10" t="s">
         <v>73</v>
       </c>
       <c r="Q2" s="10"/>
-      <c r="R2" s="49" t="s">
+      <c r="R2" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="S2" s="49" t="s">
+      <c r="S2" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="T2" s="49" t="s">
+      <c r="T2" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="U2" s="49" t="s">
+      <c r="U2" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="V2" s="49" t="s">
+      <c r="V2" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="W2" s="49" t="s">
-        <v>169</v>
-      </c>
-      <c r="X2" s="49" t="s">
-        <v>170</v>
-      </c>
-      <c r="Y2" s="49" t="s">
-        <v>171</v>
-      </c>
-      <c r="Z2" s="49" t="s">
-        <v>172</v>
+      <c r="W2" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="X2" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y2" s="48" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z2" s="48" t="s">
+        <v>167</v>
       </c>
       <c r="AA2" s="10"/>
-      <c r="AB2" s="49" t="s">
+      <c r="AB2" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="AC2" s="49" t="s">
+      <c r="AC2" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="AD2" s="49" t="s">
+      <c r="AD2" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="AE2" s="49" t="s">
+      <c r="AE2" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="AF2" s="49" t="s">
+      <c r="AF2" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="AG2" s="49" t="s">
+      <c r="AG2" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="AH2" s="49" t="s">
-        <v>102</v>
+      <c r="AH2" s="48" t="s">
+        <v>101</v>
       </c>
       <c r="AI2" s="3"/>
-      <c r="AJ2" s="47" t="s">
-        <v>82</v>
+      <c r="AJ2" s="46" t="s">
+        <v>81</v>
       </c>
       <c r="AK2" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL2" s="3" t="s">
         <v>66</v>
@@ -2499,7 +3669,7 @@
     </row>
     <row r="3" spans="1:39" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B3" s="25" t="s">
         <v>1</v>
@@ -2511,7 +3681,7 @@
         <v>61</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F3" s="24" t="s">
         <v>75</v>
@@ -2519,84 +3689,84 @@
       <c r="G3" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="49" t="s">
-        <v>79</v>
-      </c>
-      <c r="J3" s="49" t="s">
+      <c r="I3" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="K3" s="49" t="s">
+      <c r="J3" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="K3" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="L3" s="49" t="s">
+      <c r="L3" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="M3" s="53" t="s">
-        <v>104</v>
-      </c>
-      <c r="N3" s="53" t="s">
+      <c r="M3" s="52" t="s">
         <v>103</v>
+      </c>
+      <c r="N3" s="52" t="s">
+        <v>102</v>
       </c>
       <c r="O3" s="10"/>
       <c r="P3" s="10" t="s">
         <v>73</v>
       </c>
       <c r="Q3" s="10"/>
-      <c r="R3" s="49" t="s">
+      <c r="R3" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="S3" s="49" t="s">
+      <c r="S3" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="T3" s="49" t="s">
+      <c r="T3" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="U3" s="49" t="s">
+      <c r="U3" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="V3" s="49" t="s">
+      <c r="V3" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="W3" s="49" t="s">
-        <v>169</v>
-      </c>
-      <c r="X3" s="49" t="s">
-        <v>170</v>
-      </c>
-      <c r="Y3" s="49" t="s">
-        <v>171</v>
-      </c>
-      <c r="Z3" s="49" t="s">
-        <v>172</v>
+      <c r="W3" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="X3" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y3" s="48" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z3" s="48" t="s">
+        <v>167</v>
       </c>
       <c r="AA3" s="10"/>
-      <c r="AB3" s="49" t="s">
+      <c r="AB3" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="AC3" s="49" t="s">
+      <c r="AC3" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="AD3" s="49" t="s">
+      <c r="AD3" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="AE3" s="49" t="s">
+      <c r="AE3" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="AF3" s="49" t="s">
+      <c r="AF3" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="AG3" s="49" t="s">
+      <c r="AG3" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="AH3" s="49" t="s">
-        <v>102</v>
+      <c r="AH3" s="48" t="s">
+        <v>101</v>
       </c>
       <c r="AI3" s="3"/>
-      <c r="AJ3" s="47" t="s">
-        <v>82</v>
+      <c r="AJ3" s="46" t="s">
+        <v>81</v>
       </c>
       <c r="AK3" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL3" s="3" t="s">
         <v>66</v>
@@ -2608,44 +3778,44 @@
   </sheetData>
   <autoFilter ref="A1:AM3" xr:uid="{D6BF73C0-3DFA-4EF7-83FF-A6F179361B6B}"/>
   <conditionalFormatting sqref="AL2:AL65536">
-    <cfRule type="cellIs" dxfId="24" priority="24" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="24" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK2:AK65536">
-    <cfRule type="cellIs" dxfId="23" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="14" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G65536">
-    <cfRule type="beginsWith" dxfId="22" priority="1" stopIfTrue="1" operator="beginsWith" text="14">
+    <cfRule type="beginsWith" dxfId="136" priority="1" stopIfTrue="1" operator="beginsWith" text="14">
       <formula>LEFT(G2,LEN("14"))="14"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="21" priority="34" stopIfTrue="1" operator="beginsWith" text="6">
+    <cfRule type="beginsWith" dxfId="135" priority="34" stopIfTrue="1" operator="beginsWith" text="6">
       <formula>LEFT(G2,LEN("6"))="6"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="20" priority="35" stopIfTrue="1" operator="beginsWith" text="5">
+    <cfRule type="beginsWith" dxfId="134" priority="35" stopIfTrue="1" operator="beginsWith" text="5">
       <formula>LEFT(G2,LEN("5"))="5"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="19" priority="36" stopIfTrue="1" operator="beginsWith" text="4">
+    <cfRule type="beginsWith" dxfId="133" priority="36" stopIfTrue="1" operator="beginsWith" text="4">
       <formula>LEFT(G2,LEN("4"))="4"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="18" priority="71" stopIfTrue="1" operator="beginsWith" text="24">
+    <cfRule type="beginsWith" dxfId="132" priority="71" stopIfTrue="1" operator="beginsWith" text="24">
       <formula>LEFT(G2,LEN("24"))="24"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="17" priority="72" stopIfTrue="1" operator="beginsWith" text="27">
+    <cfRule type="beginsWith" dxfId="131" priority="72" stopIfTrue="1" operator="beginsWith" text="27">
       <formula>LEFT(G2,LEN("27"))="27"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="16" priority="73" stopIfTrue="1" operator="beginsWith" text="3">
+    <cfRule type="beginsWith" dxfId="130" priority="73" stopIfTrue="1" operator="beginsWith" text="3">
       <formula>LEFT(G2,LEN("3"))="3"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="15" priority="74" stopIfTrue="1" operator="beginsWith" text="23">
+    <cfRule type="beginsWith" dxfId="129" priority="74" stopIfTrue="1" operator="beginsWith" text="23">
       <formula>LEFT(G2,LEN("23"))="23"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="14" priority="75" stopIfTrue="1" operator="beginsWith" text="22">
+    <cfRule type="beginsWith" dxfId="128" priority="75" stopIfTrue="1" operator="beginsWith" text="22">
       <formula>LEFT(G2,LEN("22"))="22"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="13" priority="76" stopIfTrue="1" operator="beginsWith" text="21">
+    <cfRule type="beginsWith" dxfId="127" priority="76" stopIfTrue="1" operator="beginsWith" text="21">
       <formula>LEFT(G2,LEN("21"))="21"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2666,7 +3836,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2682,59 +3852,59 @@
     <col min="16" max="16" width="10.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="41" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:24" s="40" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="C1" s="33" t="s">
+      <c r="B1" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="44" t="s">
-        <v>84</v>
-      </c>
-      <c r="E1" s="33" t="s">
+      <c r="D1" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="44" t="s">
-        <v>84</v>
-      </c>
-      <c r="I1" s="37" t="s">
+      <c r="H1" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="J1" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="K1" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="39" t="s">
+      <c r="L1" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="M1" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="40" t="s">
+      <c r="N1" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="40" t="s">
+      <c r="O1" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="40" t="s">
+      <c r="P1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="40" t="s">
+      <c r="Q1" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="40" t="s">
+      <c r="R1" s="39" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2743,10 +3913,10 @@
         <v>69</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="4" t="s">
@@ -2813,9 +3983,9 @@
   </sheetPr>
   <dimension ref="A1:AI5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
+      <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2846,69 +4016,69 @@
     <col min="24" max="16384" width="11.42578125" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="54" customFormat="1" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="55"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="G1" s="36" t="s">
-        <v>161</v>
-      </c>
-      <c r="H1" s="36" t="s">
-        <v>159</v>
-      </c>
-      <c r="I1" s="36" t="s">
-        <v>160</v>
-      </c>
-      <c r="J1" s="36" t="s">
+    <row r="1" spans="1:35" s="53" customFormat="1" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="54"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="H1" s="35" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="J1" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="L1" s="31" t="s">
+      <c r="K1" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="L1" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="M1" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="M1" s="31" t="s">
+      <c r="N1" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="N1" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="O1" s="32" t="s">
+      <c r="O1" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="42" t="s">
-        <v>84</v>
+      <c r="P1" s="41" t="s">
+        <v>83</v>
       </c>
       <c r="Q1" s="90" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R1" s="91"/>
       <c r="S1" s="92"/>
-      <c r="T1" s="42" t="s">
-        <v>84</v>
+      <c r="T1" s="41" t="s">
+        <v>83</v>
       </c>
       <c r="U1" s="90" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="V1" s="93"/>
       <c r="W1" s="94"/>
-      <c r="X1" s="57"/>
+      <c r="X1" s="56"/>
       <c r="Y1" s="90" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="Z1" s="93"/>
       <c r="AA1" s="94"/>
       <c r="AB1" s="90" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="AC1" s="93"/>
       <c r="AD1" s="93"/>
-      <c r="AE1" s="42" t="s">
-        <v>84</v>
+      <c r="AE1" s="41" t="s">
+        <v>83</v>
       </c>
       <c r="AF1" s="95" t="s">
         <v>44</v>
@@ -2916,84 +4086,84 @@
       <c r="AG1" s="91"/>
       <c r="AH1" s="92"/>
     </row>
-    <row r="2" spans="1:35" s="54" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="55"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="59"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="42"/>
+    <row r="2" spans="1:35" s="53" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="54"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="41"/>
       <c r="Q2" s="19"/>
       <c r="R2" s="16"/>
       <c r="S2" s="17"/>
-      <c r="T2" s="42"/>
-      <c r="U2" s="61"/>
-      <c r="V2" s="62"/>
-      <c r="W2" s="63"/>
-      <c r="X2" s="57"/>
-      <c r="Y2" s="77"/>
-      <c r="Z2" s="80"/>
-      <c r="AA2" s="66"/>
-      <c r="AB2" s="77"/>
-      <c r="AC2" s="80"/>
-      <c r="AD2" s="66"/>
-      <c r="AE2" s="42"/>
+      <c r="T2" s="41"/>
+      <c r="U2" s="60"/>
+      <c r="V2" s="61"/>
+      <c r="W2" s="62"/>
+      <c r="X2" s="56"/>
+      <c r="Y2" s="76"/>
+      <c r="Z2" s="79"/>
+      <c r="AA2" s="65"/>
+      <c r="AB2" s="76"/>
+      <c r="AC2" s="79"/>
+      <c r="AD2" s="65"/>
+      <c r="AE2" s="41"/>
       <c r="AF2" s="19"/>
       <c r="AG2" s="16"/>
       <c r="AH2" s="17"/>
     </row>
-    <row r="3" spans="1:35" s="67" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="64" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="89" t="s">
+    <row r="3" spans="1:35" s="66" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="88" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="88" t="s">
         <v>111</v>
       </c>
-      <c r="E3" s="89" t="s">
+      <c r="F3" s="81" t="s">
         <v>112</v>
       </c>
-      <c r="F3" s="82" t="s">
+      <c r="G3" s="81" t="s">
         <v>113</v>
       </c>
-      <c r="G3" s="82" t="s">
+      <c r="H3" s="81" t="s">
         <v>114</v>
       </c>
-      <c r="H3" s="82" t="s">
+      <c r="I3" s="81" t="s">
         <v>115</v>
       </c>
-      <c r="I3" s="82" t="s">
+      <c r="J3" s="81" t="s">
         <v>116</v>
       </c>
-      <c r="J3" s="82" t="s">
+      <c r="K3" s="82" t="s">
         <v>117</v>
       </c>
-      <c r="K3" s="83" t="s">
+      <c r="L3" s="83" t="s">
         <v>118</v>
       </c>
-      <c r="L3" s="84" t="s">
+      <c r="M3" s="84" t="s">
         <v>119</v>
       </c>
-      <c r="M3" s="85" t="s">
+      <c r="N3" s="84" t="s">
         <v>120</v>
       </c>
-      <c r="N3" s="85" t="s">
+      <c r="O3" s="85" t="s">
         <v>121</v>
       </c>
-      <c r="O3" s="86" t="s">
+      <c r="P3" s="86" t="s">
         <v>122</v>
-      </c>
-      <c r="P3" s="87" t="s">
-        <v>123</v>
       </c>
       <c r="Q3" s="19" t="s">
         <v>67</v>
@@ -3002,10 +4172,10 @@
         <v>68</v>
       </c>
       <c r="S3" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="T3" s="87" t="s">
-        <v>124</v>
+        <v>112</v>
+      </c>
+      <c r="T3" s="86" t="s">
+        <v>123</v>
       </c>
       <c r="U3" s="19" t="s">
         <v>67</v>
@@ -3014,31 +4184,31 @@
         <v>68</v>
       </c>
       <c r="W3" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="X3" s="88" t="s">
+        <v>112</v>
+      </c>
+      <c r="X3" s="87" t="s">
+        <v>124</v>
+      </c>
+      <c r="Y3" s="80" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z3" s="77" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA3" s="65" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB3" s="77" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC3" s="78" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD3" s="65" t="s">
+        <v>112</v>
+      </c>
+      <c r="AE3" s="86" t="s">
         <v>125</v>
-      </c>
-      <c r="Y3" s="81" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z3" s="78" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA3" s="66" t="s">
-        <v>113</v>
-      </c>
-      <c r="AB3" s="78" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC3" s="79" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD3" s="66" t="s">
-        <v>113</v>
-      </c>
-      <c r="AE3" s="87" t="s">
-        <v>126</v>
       </c>
       <c r="AF3" s="19" t="s">
         <v>67</v>
@@ -3047,114 +4217,114 @@
         <v>68</v>
       </c>
       <c r="AH3" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:35" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="54" t="s">
-        <v>142</v>
-      </c>
-      <c r="C4" s="55"/>
+    <row r="4" spans="1:35" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="53" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="54"/>
       <c r="D4" s="8" t="s">
         <v>71</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F4" s="68" t="s">
+      <c r="F4" s="67" t="s">
+        <v>135</v>
+      </c>
+      <c r="G4" s="67" t="s">
+        <v>132</v>
+      </c>
+      <c r="H4" s="67" t="s">
         <v>136</v>
       </c>
-      <c r="G4" s="68" t="s">
+      <c r="I4" s="67" t="s">
         <v>133</v>
       </c>
-      <c r="H4" s="68" t="s">
+      <c r="J4" s="67" t="s">
+        <v>134</v>
+      </c>
+      <c r="K4" s="68"/>
+      <c r="L4" s="69"/>
+      <c r="M4" s="69"/>
+      <c r="N4" s="69"/>
+      <c r="O4" s="69"/>
+      <c r="P4" s="70"/>
+      <c r="Q4" s="69">
+        <v>1</v>
+      </c>
+      <c r="R4" s="72" t="s">
         <v>137</v>
       </c>
-      <c r="I4" s="68" t="s">
-        <v>134</v>
-      </c>
-      <c r="J4" s="68" t="s">
-        <v>135</v>
-      </c>
-      <c r="K4" s="69"/>
-      <c r="L4" s="70"/>
-      <c r="M4" s="70"/>
-      <c r="N4" s="70"/>
-      <c r="O4" s="70"/>
-      <c r="P4" s="71"/>
-      <c r="Q4" s="70">
+      <c r="S4" s="67" t="s">
+        <v>130</v>
+      </c>
+      <c r="T4" s="69"/>
+      <c r="U4" s="69" t="s">
+        <v>157</v>
+      </c>
+      <c r="V4" s="69" t="s">
+        <v>131</v>
+      </c>
+      <c r="W4" s="69" t="s">
+        <v>129</v>
+      </c>
+      <c r="X4" s="69"/>
+      <c r="Y4" s="69" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z4" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="AA4" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB4" s="69" t="s">
+        <v>159</v>
+      </c>
+      <c r="AC4" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD4" s="67" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE4" s="71"/>
+      <c r="AF4" s="69">
         <v>1</v>
       </c>
-      <c r="R4" s="73" t="s">
+      <c r="AG4" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="S4" s="70" t="s">
-        <v>131</v>
-      </c>
-      <c r="T4" s="70"/>
-      <c r="U4" s="70" t="s">
-        <v>162</v>
-      </c>
-      <c r="V4" s="70" t="s">
-        <v>132</v>
-      </c>
-      <c r="W4" s="70" t="s">
-        <v>130</v>
-      </c>
-      <c r="X4" s="70"/>
-      <c r="Y4" s="70" t="s">
-        <v>163</v>
-      </c>
-      <c r="Z4" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="AA4" s="70" t="s">
-        <v>129</v>
-      </c>
-      <c r="AB4" s="70" t="s">
-        <v>164</v>
-      </c>
-      <c r="AC4" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="AD4" s="70" t="s">
-        <v>128</v>
-      </c>
-      <c r="AE4" s="72"/>
-      <c r="AF4" s="70">
-        <v>1</v>
-      </c>
-      <c r="AG4" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="AH4" s="70" t="s">
-        <v>127</v>
+      <c r="AH4" s="67" t="s">
+        <v>126</v>
       </c>
       <c r="AI4" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:35" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="55"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
+    <row r="5" spans="1:35" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="54"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
       <c r="F5" s="25"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="56"/>
-      <c r="K5" s="56"/>
-      <c r="L5" s="56"/>
-      <c r="M5" s="56"/>
-      <c r="N5" s="56"/>
-      <c r="O5" s="56"/>
-      <c r="P5" s="56"/>
-      <c r="Q5" s="56"/>
-      <c r="R5" s="56"/>
-      <c r="S5" s="56"/>
-      <c r="T5" s="56"/>
-      <c r="U5" s="56"/>
-      <c r="V5" s="56"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="55"/>
+      <c r="K5" s="55"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="55"/>
+      <c r="N5" s="55"/>
+      <c r="O5" s="55"/>
+      <c r="P5" s="55"/>
+      <c r="Q5" s="55"/>
+      <c r="R5" s="55"/>
+      <c r="S5" s="55"/>
+      <c r="T5" s="55"/>
+      <c r="U5" s="55"/>
+      <c r="V5" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3164,56 +4334,48 @@
     <mergeCell ref="AB1:AD1"/>
     <mergeCell ref="AF1:AH1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E5 V6:V1002 O6:O1002 K6:K1002">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="lessThan">
+  <conditionalFormatting sqref="F4:F65536">
+    <cfRule type="cellIs" dxfId="17" priority="9" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q6:R1002">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
-      <formula>"Pas OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E2">
-    <cfRule type="cellIs" dxfId="10" priority="9" operator="lessThan">
+  <conditionalFormatting sqref="G4:G65536">
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="lessThan">
+  <conditionalFormatting sqref="H4:H65536">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V5 O5 K5">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="lessThan">
+  <conditionalFormatting sqref="I4:I65536">
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q5:R5">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
-      <formula>"Pas OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F4:J5">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="J4:J65536">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA4:AB4 AH4 AD4:AF4">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThan">
+  <conditionalFormatting sqref="S4:S65536">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q4 S4:Y4 AH4 AA4:AB4 AD4:AF4">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+  <conditionalFormatting sqref="AA4:AA65536">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA4:AB4 AH4 AD4:AF4">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+  <conditionalFormatting sqref="AD4:AD65536">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH4:AH65536">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3228,13 +4390,13 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:AL16"/>
+  <dimension ref="A1:AN8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3245,10 +4407,10 @@
     <col min="4" max="4" width="13.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" style="2" customWidth="1"/>
     <col min="6" max="6" width="6.5703125" style="26" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" style="2" customWidth="1"/>
     <col min="9" max="9" width="10.42578125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="2" customWidth="1"/>
     <col min="11" max="11" width="8.140625" style="2" customWidth="1"/>
     <col min="12" max="12" width="2.85546875" style="2" customWidth="1"/>
     <col min="13" max="13" width="16.28515625" style="2" customWidth="1"/>
@@ -3256,122 +4418,132 @@
     <col min="15" max="15" width="10.140625" style="2" customWidth="1"/>
     <col min="16" max="16" width="7.42578125" style="2" customWidth="1"/>
     <col min="17" max="17" width="8.7109375" style="2" customWidth="1"/>
-    <col min="18" max="18" width="8.7109375" style="26" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="9.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.28515625" style="2" customWidth="1"/>
-    <col min="26" max="27" width="9.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" style="102" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.42578125" style="102" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.7109375" style="102" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7" style="26" customWidth="1"/>
+    <col min="24" max="24" width="7.85546875" style="26" customWidth="1"/>
+    <col min="26" max="26" width="9.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.140625" style="26" customWidth="1"/>
+    <col min="29" max="29" width="4.85546875" style="25" customWidth="1"/>
+    <col min="30" max="30" width="9.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.5703125" style="26" customWidth="1"/>
+    <col min="34" max="34" width="9.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="6.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="4.85546875" style="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="7" customFormat="1" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40" s="7" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="96"/>
       <c r="B1" s="97"/>
       <c r="C1" s="97"/>
       <c r="D1" s="97"/>
       <c r="E1" s="98"/>
       <c r="F1" s="26"/>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="36" t="s">
-        <v>109</v>
-      </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="M1" s="31" t="s">
+      <c r="L1" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M1" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="N1" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="N1" s="31" t="s">
+      <c r="O1" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="O1" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="P1" s="32" t="s">
+      <c r="P1" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="42" t="s">
-        <v>84</v>
+      <c r="Q1" s="41" t="s">
+        <v>83</v>
       </c>
       <c r="R1" s="95" t="s">
         <v>63</v>
       </c>
       <c r="S1" s="91"/>
       <c r="T1" s="92"/>
-      <c r="U1" s="42"/>
+      <c r="U1" s="41" t="s">
+        <v>83</v>
+      </c>
       <c r="V1" s="90" t="s">
-        <v>156</v>
-      </c>
-      <c r="W1" s="91"/>
-      <c r="X1" s="92"/>
-      <c r="Y1" s="42" t="s">
-        <v>84</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="W1" s="93"/>
+      <c r="X1" s="94"/>
+      <c r="Y1" s="56"/>
       <c r="Z1" s="90" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="AA1" s="93"/>
       <c r="AB1" s="94"/>
-      <c r="AC1" s="42" t="s">
-        <v>84</v>
-      </c>
+      <c r="AC1" s="89"/>
       <c r="AD1" s="90" t="s">
-        <v>154</v>
+        <v>170</v>
       </c>
       <c r="AE1" s="93"/>
       <c r="AF1" s="94"/>
-      <c r="AG1" s="25"/>
+      <c r="AG1" s="41" t="s">
+        <v>83</v>
+      </c>
       <c r="AH1" s="95" t="s">
         <v>44</v>
       </c>
       <c r="AI1" s="91"/>
       <c r="AJ1" s="92"/>
+      <c r="AL1" s="103" t="s">
+        <v>177</v>
+      </c>
     </row>
-    <row r="2" spans="1:38" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
+    <row r="2" spans="1:40" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="36" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="36" t="s">
+      <c r="B2" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="35" t="s">
         <v>20</v>
       </c>
       <c r="F2" s="26"/>
-      <c r="G2" s="82" t="s">
+      <c r="G2" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="81" t="s">
         <v>113</v>
       </c>
-      <c r="H2" s="82" t="s">
+      <c r="I2" s="81" t="s">
         <v>114</v>
       </c>
-      <c r="I2" s="82" t="s">
+      <c r="J2" s="81" t="s">
         <v>115</v>
       </c>
-      <c r="J2" s="82" t="s">
+      <c r="K2" s="81" t="s">
         <v>116</v>
-      </c>
-      <c r="K2" s="82" t="s">
-        <v>117</v>
       </c>
       <c r="L2" s="18"/>
       <c r="M2" s="19"/>
@@ -3386,82 +4558,90 @@
         <v>68</v>
       </c>
       <c r="T2" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="U2" s="86" t="s">
+        <v>123</v>
+      </c>
+      <c r="V2" s="99" t="s">
+        <v>67</v>
+      </c>
+      <c r="W2" s="99" t="s">
+        <v>68</v>
+      </c>
+      <c r="X2" s="99" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y2" s="87" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z2" s="99" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA2" s="99" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB2" s="99" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC2" s="87" t="s">
+        <v>124</v>
+      </c>
+      <c r="AD2" s="99" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE2" s="99" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF2" s="99" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG2" s="87" t="s">
+        <v>125</v>
+      </c>
+      <c r="AH2" s="99" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI2" s="99" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ2" s="99" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="73" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="74" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="67" t="s">
         <v>76</v>
       </c>
-      <c r="U2" s="20"/>
-      <c r="V2" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="W2" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="X2" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA2" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB2" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="AC2" s="20"/>
-      <c r="AD2" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="AE2" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF2" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="AG2" s="25"/>
-      <c r="AH2" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="AI2" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="AJ2" s="23" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:38" s="74" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="74" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" s="75" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="68" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="68" t="s">
+      <c r="E3" s="67" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="8"/>
-      <c r="G3" s="54" t="s">
+      <c r="G3" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="K3" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="J3" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="L3" s="69"/>
+      <c r="L3" s="68"/>
       <c r="M3" s="8" t="s">
         <v>35</v>
       </c>
@@ -3475,66 +4655,121 @@
         <v>28</v>
       </c>
       <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
+      <c r="R3" s="100" t="s">
+        <v>176</v>
+      </c>
+      <c r="S3" s="101" t="s">
+        <v>35</v>
+      </c>
       <c r="T3" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="V3" s="69" t="s">
+        <v>178</v>
+      </c>
+      <c r="W3" s="100" t="s">
+        <v>173</v>
+      </c>
+      <c r="X3" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8" t="s">
+      <c r="Z3" s="69" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA3" s="69" t="s">
+        <v>174</v>
+      </c>
+      <c r="AB3" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="AC3" s="8"/>
-      <c r="AD3" s="8"/>
-      <c r="AE3" s="8"/>
+      <c r="AD3" s="69" t="s">
+        <v>180</v>
+      </c>
+      <c r="AE3" s="8" t="s">
+        <v>175</v>
+      </c>
       <c r="AF3" s="8" t="s">
-        <v>146</v>
+        <v>171</v>
       </c>
       <c r="AH3" s="8">
         <v>1</v>
       </c>
-      <c r="AI3" s="8" t="s">
-        <v>152</v>
+      <c r="AI3" s="72" t="s">
+        <v>150</v>
       </c>
       <c r="AJ3" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="AL3" s="76" t="s">
+        <v>172</v>
+      </c>
+      <c r="AN3" s="75" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="P8" s="26"/>
-    </row>
-    <row r="16" spans="1:38" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="S16" s="28"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:E2" xr:uid="{69864F3B-0295-46A6-855E-10D8CEC02147}"/>
   <mergeCells count="6">
-    <mergeCell ref="R1:T1"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="AH1:AJ1"/>
-    <mergeCell ref="V1:X1"/>
     <mergeCell ref="Z1:AB1"/>
     <mergeCell ref="AD1:AF1"/>
+    <mergeCell ref="R1:T1"/>
+    <mergeCell ref="V1:X1"/>
   </mergeCells>
-  <conditionalFormatting sqref="O10:O1000 S15 AA4:AA1000 T4:T1000 O4:O8">
-    <cfRule type="cellIs" dxfId="1" priority="19" stopIfTrue="1" operator="greaterThan">
+  <conditionalFormatting sqref="O4:O65536">
+    <cfRule type="cellIs" dxfId="50" priority="43" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V4:W1000 AD3:AE3">
-    <cfRule type="cellIs" dxfId="0" priority="15" stopIfTrue="1" operator="equal">
-      <formula>"Pas OK"</formula>
+  <conditionalFormatting sqref="T3:T65536">
+    <cfRule type="cellIs" dxfId="49" priority="14" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X3:X65536">
+    <cfRule type="cellIs" dxfId="48" priority="13" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB3:AB65536">
+    <cfRule type="cellIs" dxfId="47" priority="12" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF3:AF65536">
+    <cfRule type="cellIs" dxfId="40" priority="11" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ3:AJ65536">
+    <cfRule type="cellIs" dxfId="41" priority="10" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G65536">
+    <cfRule type="cellIs" dxfId="46" priority="5" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H65536">
+    <cfRule type="cellIs" dxfId="45" priority="4" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I65536">
+    <cfRule type="cellIs" dxfId="44" priority="3" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J65536">
+    <cfRule type="cellIs" dxfId="43" priority="2" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K65536">
+    <cfRule type="cellIs" dxfId="42" priority="1" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3556,19 +4791,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>81</v>
+      <c r="A1" s="28" t="s">
+        <v>80</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" s="29"/>
+        <v>79</v>
+      </c>
+      <c r="C1" s="28"/>
     </row>
     <row r="2" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="29" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3585,9 +4820,7 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3599,7 +4832,7 @@
       <c r="A1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="46">
+      <c r="B1" s="45">
         <v>43477</v>
       </c>
     </row>
@@ -3613,10 +4846,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="25" t="s">
         <v>97</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -3631,7 +4864,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Corrections de quotas #9
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele.xlsx
+++ b/fichiers/conf/modele.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B00F34-66CC-47A5-8A69-2AD92291DC87}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B2F577-516F-451B-A947-3A7D91C9D2A5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3360" yWindow="0" windowWidth="28800" windowHeight="11625" tabRatio="466" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
@@ -861,20 +861,9 @@
     <t>${unite.psc1afps}</t>
   </si>
   <si>
-    <t>Encadrement 2ème étape
-par rapport au minimum d'animateurs : 
-80% titulaire ou stagiaire +
-1 dir titulaire</t>
-  </si>
-  <si>
     <t>Encadrement 1ère étape
 1 animateur pour 12 jeunes
 plus directeur</t>
-  </si>
-  <si>
-    <t>Encadrement 2ème étape
-par rapport au minimum d'animateurs : 
-50% titulaire + 1 dir titulaire</t>
   </si>
   <si>
     <t>Nb titulaires et 1 dir</t>
@@ -978,39 +967,12 @@
     <t>Delta1</t>
   </si>
   <si>
-    <t>$[T4]</t>
-  </si>
-  <si>
-    <t>$[X4]</t>
-  </si>
-  <si>
-    <t>$[AB4]</t>
-  </si>
-  <si>
-    <t>$[AF4]</t>
-  </si>
-  <si>
-    <t>$[AJ4]</t>
-  </si>
-  <si>
-    <t>$[IF($B4=$C4,0,1)]</t>
-  </si>
-  <si>
     <t>$[N4-M4]</t>
   </si>
   <si>
-    <t>$[CEILING($D4/12,1)+IF((VALUE(C4)-VALUE(B4))/10=3,0,1)]</t>
-  </si>
-  <si>
-    <t>$[CEILING($D4*0.5/12,1)+IF((VALUE(C4)-VALUE(B4))/10=3,0,1)]</t>
-  </si>
-  <si>
     <t>$[V4-Q4]</t>
   </si>
   <si>
-    <t>$[CEILING($D4*0.8/12,1)+IF((VALUE(C4)-VALUE(B4))/10=3,0,1)]</t>
-  </si>
-  <si>
     <t>$[AD4-AC4]&lt;/jt:forEach&gt;</t>
   </si>
   <si>
@@ -1021,6 +983,44 @@
   </si>
   <si>
     <t>${unite.object.dirsfqnonq}</t>
+  </si>
+  <si>
+    <t>Encadrement 2ème étape
+par rapport au minimum d'animateurs : 
+50% titulaire + 1 dir titulaire hors compagnons</t>
+  </si>
+  <si>
+    <t>Encadrement 2ème étape
+par rapport au minimum d'animateurs : 
+80% titulaire ou stagiaire +
+1 dir titulaire ou stagiaire hors compagnons</t>
+  </si>
+  <si>
+    <t>$[O4]</t>
+  </si>
+  <si>
+    <t>$[S4]</t>
+  </si>
+  <si>
+    <t>$[W4]</t>
+  </si>
+  <si>
+    <t>$[AA4]</t>
+  </si>
+  <si>
+    <t>$[AE4]</t>
+  </si>
+  <si>
+    <t>$[IF($B4=$C4,0,IF(ROUND((VALUE(C4)-VALUE(B4))/10,0)=4,0,1))]</t>
+  </si>
+  <si>
+    <t>$[CEILING($D4/12,1)+IF(ROUND((VALUE(C4)-VALUE(B4))/10,0)=3,0,1)]</t>
+  </si>
+  <si>
+    <t>$[CEILING($D4*0.5/12,1)+IF(ROUND((VALUE(C4)-VALUE(B4))/10,0)=3,0,1)]</t>
+  </si>
+  <si>
+    <t>$[CEILING($D4*0.8/12,1)+IF(ROUND((VALUE(C4)-VALUE(B4))/10,0)=3,0,1)]</t>
   </si>
 </sst>
 </file>
@@ -2240,16 +2240,16 @@
         <v>12</v>
       </c>
       <c r="W1" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="X1" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y1" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="X1" s="39" t="s">
+      <c r="Z1" s="39" t="s">
         <v>123</v>
-      </c>
-      <c r="Y1" s="39" t="s">
-        <v>124</v>
-      </c>
-      <c r="Z1" s="39" t="s">
-        <v>125</v>
       </c>
       <c r="AA1" s="31" t="s">
         <v>78</v>
@@ -2349,16 +2349,16 @@
         <v>48</v>
       </c>
       <c r="W2" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="X2" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="Y2" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="X2" s="38" t="s">
+      <c r="Z2" s="38" t="s">
         <v>127</v>
-      </c>
-      <c r="Y2" s="38" t="s">
-        <v>128</v>
-      </c>
-      <c r="Z2" s="38" t="s">
-        <v>129</v>
       </c>
       <c r="AA2" s="10"/>
       <c r="AB2" s="38" t="s">
@@ -2390,7 +2390,7 @@
         <v>90</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:38" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -2454,16 +2454,16 @@
         <v>48</v>
       </c>
       <c r="W3" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="X3" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="Y3" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="X3" s="38" t="s">
+      <c r="Z3" s="38" t="s">
         <v>127</v>
-      </c>
-      <c r="Y3" s="38" t="s">
-        <v>128</v>
-      </c>
-      <c r="Z3" s="38" t="s">
-        <v>129</v>
       </c>
       <c r="AA3" s="10"/>
       <c r="AB3" s="38" t="s">
@@ -2495,7 +2495,7 @@
         <v>90</v>
       </c>
       <c r="AL3" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2707,10 +2707,10 @@
   <dimension ref="A1:AC5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="L4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2737,7 +2737,7 @@
     <col min="22" max="22" width="8.42578125" style="17" customWidth="1"/>
     <col min="23" max="23" width="11.42578125" style="17"/>
     <col min="24" max="24" width="9" style="17" customWidth="1"/>
-    <col min="25" max="25" width="8.85546875" style="17" customWidth="1"/>
+    <col min="25" max="25" width="15.85546875" style="17" customWidth="1"/>
     <col min="26" max="26" width="3.140625" style="17" customWidth="1"/>
     <col min="27" max="27" width="11.42578125" style="17"/>
     <col min="28" max="28" width="10.140625" style="17" customWidth="1"/>
@@ -2753,13 +2753,13 @@
         <v>97</v>
       </c>
       <c r="G1" s="25" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H1" s="25" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I1" s="25" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J1" s="25" t="s">
         <v>27</v>
@@ -2776,18 +2776,18 @@
         <v>78</v>
       </c>
       <c r="P1" s="76" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Q1" s="79"/>
       <c r="R1" s="80"/>
       <c r="S1" s="46"/>
       <c r="T1" s="76" t="s">
-        <v>118</v>
+        <v>154</v>
       </c>
       <c r="U1" s="79"/>
       <c r="V1" s="80"/>
       <c r="W1" s="79" t="s">
-        <v>116</v>
+        <v>155</v>
       </c>
       <c r="X1" s="79"/>
       <c r="Y1" s="80"/>
@@ -2842,7 +2842,7 @@
         <v>103</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G3" s="25" t="s">
         <v>105</v>
@@ -2916,7 +2916,7 @@
     </row>
     <row r="4" spans="1:29" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C4" s="44"/>
       <c r="D4" s="8" t="s">
@@ -2926,58 +2926,58 @@
         <v>58</v>
       </c>
       <c r="F4" s="51" t="s">
+        <v>142</v>
+      </c>
+      <c r="G4" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="H4" s="51" t="s">
         <v>144</v>
       </c>
-      <c r="G4" s="51" t="s">
+      <c r="I4" s="51" t="s">
         <v>145</v>
       </c>
-      <c r="H4" s="51" t="s">
+      <c r="J4" s="51" t="s">
         <v>146</v>
-      </c>
-      <c r="I4" s="51" t="s">
-        <v>147</v>
-      </c>
-      <c r="J4" s="51" t="s">
-        <v>148</v>
       </c>
       <c r="K4" s="52"/>
       <c r="L4" s="53">
         <v>1</v>
       </c>
       <c r="M4" s="55" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="N4" s="51" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="O4" s="53"/>
       <c r="P4" s="53" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="Q4" s="53" t="s">
         <v>111</v>
       </c>
       <c r="R4" s="53" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S4" s="53"/>
       <c r="T4" s="53" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="U4" s="8" t="s">
         <v>113</v>
       </c>
       <c r="V4" s="51" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="W4" s="53" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="X4" s="8" t="s">
         <v>114</v>
       </c>
       <c r="Y4" s="51" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="Z4" s="54"/>
       <c r="AA4" s="53">
@@ -2987,7 +2987,7 @@
         <v>112</v>
       </c>
       <c r="AC4" s="51" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:29" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -3077,7 +3077,7 @@
       <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" sqref="A1:E1"/>
+      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3123,7 +3123,7 @@
       <c r="E1" s="84"/>
       <c r="F1" s="18"/>
       <c r="G1" s="25" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="H1" s="25" t="s">
         <v>98</v>
@@ -3149,19 +3149,19 @@
         <v>78</v>
       </c>
       <c r="Q1" s="76" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="R1" s="79"/>
       <c r="S1" s="80"/>
       <c r="T1" s="46"/>
       <c r="U1" s="76" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="V1" s="79"/>
       <c r="W1" s="80"/>
       <c r="X1" s="71"/>
       <c r="Y1" s="76" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="Z1" s="79"/>
       <c r="AA1" s="80"/>
@@ -3320,32 +3320,32 @@
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="L4" s="52"/>
       <c r="M4" s="60" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="N4" s="61" t="s">
         <v>33</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="Q4" s="53" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="R4" s="60" t="s">
         <v>111</v>
@@ -3354,19 +3354,19 @@
         <v>110</v>
       </c>
       <c r="U4" s="53" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="V4" s="53" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="Y4" s="53" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="Z4" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AA4" s="8" t="s">
         <v>109</v>
@@ -3378,7 +3378,7 @@
         <v>115</v>
       </c>
       <c r="AE4" s="8" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correction de calcul de deltas
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele.xlsx
+++ b/fichiers/conf/modele.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC09AE9D-C0E4-4EE0-9529-742C8C829F5F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C891250-41FB-45DD-8589-291698652CED}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="0" windowWidth="28800" windowHeight="11625" tabRatio="524" activeTab="3" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="1290" yWindow="795" windowWidth="23145" windowHeight="13935" tabRatio="566" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Responsables" sheetId="1" r:id="rId1"/>
@@ -940,9 +940,6 @@
     <t>$[N4-M4]</t>
   </si>
   <si>
-    <t>$[V4-Q4]</t>
-  </si>
-  <si>
     <t>$[AD4-AC4]&lt;/jt:forEach&gt;</t>
   </si>
   <si>
@@ -1020,6 +1017,9 @@
 par rapport au minimum d'animateurs : 
 80% titulaire ou stagiaire +
 1 dir titulaire (sauf rouge)</t>
+  </si>
+  <si>
+    <t>$[V4-U4]</t>
   </si>
 </sst>
 </file>
@@ -2129,7 +2129,7 @@
   </sheetPr>
   <dimension ref="A1:AL3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2741,7 +2741,7 @@
       <c r="D1" s="45"/>
       <c r="E1" s="45"/>
       <c r="F1" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G1" s="25" t="s">
         <v>115</v>
@@ -2773,12 +2773,12 @@
       <c r="R1" s="77"/>
       <c r="S1" s="46"/>
       <c r="T1" s="73" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="U1" s="76"/>
       <c r="V1" s="77"/>
       <c r="W1" s="76" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X1" s="76"/>
       <c r="Y1" s="77"/>
@@ -2907,7 +2907,7 @@
     </row>
     <row r="4" spans="1:29" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C4" s="44"/>
       <c r="D4" s="8" t="s">
@@ -2936,7 +2936,7 @@
         <v>1</v>
       </c>
       <c r="M4" s="53" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N4" s="49" t="s">
         <v>130</v>
@@ -3064,11 +3064,11 @@
   </sheetPr>
   <dimension ref="A1:AE4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" sqref="A1:E1"/>
+      <selection pane="bottomRight" activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3114,16 +3114,16 @@
       <c r="E1" s="81"/>
       <c r="F1" s="18"/>
       <c r="G1" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="J1" s="25" t="s">
         <v>158</v>
-      </c>
-      <c r="H1" s="25" t="s">
-        <v>160</v>
-      </c>
-      <c r="I1" s="25" t="s">
-        <v>161</v>
-      </c>
-      <c r="J1" s="25" t="s">
-        <v>159</v>
       </c>
       <c r="K1" s="25" t="s">
         <v>27</v>
@@ -3140,19 +3140,19 @@
         <v>78</v>
       </c>
       <c r="Q1" s="73" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="R1" s="76"/>
       <c r="S1" s="77"/>
       <c r="T1" s="46"/>
       <c r="U1" s="73" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="V1" s="76"/>
       <c r="W1" s="77"/>
       <c r="X1" s="68"/>
       <c r="Y1" s="73" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Z1" s="76"/>
       <c r="AA1" s="77"/>
@@ -3311,23 +3311,23 @@
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="I4" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="J4" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="K4" s="8" t="s">
         <v>152</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>153</v>
       </c>
       <c r="L4" s="50"/>
       <c r="M4" s="57" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N4" s="58" t="s">
         <v>33</v>
@@ -3336,7 +3336,7 @@
         <v>141</v>
       </c>
       <c r="Q4" s="51" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="R4" s="57" t="s">
         <v>107</v>
@@ -3345,16 +3345,16 @@
         <v>106</v>
       </c>
       <c r="U4" s="51" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="V4" s="51" t="s">
         <v>124</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>142</v>
+        <v>164</v>
       </c>
       <c r="Y4" s="51" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Z4" s="8" t="s">
         <v>125</v>
@@ -3369,7 +3369,7 @@
         <v>111</v>
       </c>
       <c r="AE4" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Affichage des MODULE APPRO, MODULE ANIMATEUR et APPRO Surveillant de Baignade
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele.xlsx
+++ b/fichiers/conf/modele.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C891250-41FB-45DD-8589-291698652CED}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2D84A9-A98F-4E49-AB4D-9B330BBFB84A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1290" yWindow="795" windowWidth="23145" windowHeight="13935" tabRatio="566" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="477" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Responsables" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,8 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Quotas Année'!$A$3:$AC$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Quotas Camps'!$A$3:$AE$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Responsables!$A$1:$AL$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Synthèse par unité'!$A$1:$R$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Responsables!$A$1:$AQ$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Synthèse par unité'!$A$1:$Y$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -216,7 +216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{6045E9B0-AA1D-41B4-9C3C-BC746D9BC589}">
+    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{83C77407-EDE7-4503-93FD-393628AE54E4}">
       <text>
         <r>
           <rPr>
@@ -240,7 +240,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{1F3E1ACB-E2A6-4A98-A36E-7ABE327D55F6}">
+    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{83CCAF6B-404B-4C1D-92E5-BE497427DD7D}">
       <text>
         <r>
           <rPr>
@@ -264,7 +264,113 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{D7CCADB1-4D8A-4BC8-905C-D1BA438E77F1}">
+    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{156BCBB7-1FAF-413C-8ECC-A4A9CA20E3FD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Sébastien:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fin de stage</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{2C5F74EA-D518-4557-AC0F-8BFFC404907C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sébastien:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fin de stage</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{6045E9B0-AA1D-41B4-9C3C-BC746D9BC589}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sébastien:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fin de stage</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{1F3E1ACB-E2A6-4A98-A36E-7ABE327D55F6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sébastien:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fin de stage</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AG1" authorId="0" shapeId="0" xr:uid="{D7CCADB1-4D8A-4BC8-905C-D1BA438E77F1}">
       <text>
         <r>
           <rPr>
@@ -288,7 +394,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="0" shapeId="0" xr:uid="{E9756D3C-D426-47A5-A95D-19409772C521}">
+    <comment ref="AH1" authorId="0" shapeId="0" xr:uid="{E9756D3C-D426-47A5-A95D-19409772C521}">
       <text>
         <r>
           <rPr>
@@ -312,7 +418,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD1" authorId="0" shapeId="0" xr:uid="{2F31B678-BEA5-4DB4-AC1D-AC1EC879D750}">
+    <comment ref="AI1" authorId="0" shapeId="0" xr:uid="{2F31B678-BEA5-4DB4-AC1D-AC1EC879D750}">
       <text>
         <r>
           <rPr>
@@ -336,7 +442,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE1" authorId="0" shapeId="0" xr:uid="{C8A48C2F-9EB4-4B10-8DBC-DE0A2B010CD5}">
+    <comment ref="AJ1" authorId="0" shapeId="0" xr:uid="{C8A48C2F-9EB4-4B10-8DBC-DE0A2B010CD5}">
       <text>
         <r>
           <rPr>
@@ -360,7 +466,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF1" authorId="0" shapeId="0" xr:uid="{CE08BEFE-EAC8-4844-983C-8BADEFBFE2C5}">
+    <comment ref="AK1" authorId="0" shapeId="0" xr:uid="{CE08BEFE-EAC8-4844-983C-8BADEFBFE2C5}">
       <text>
         <r>
           <rPr>
@@ -384,7 +490,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG1" authorId="0" shapeId="0" xr:uid="{28DEFE86-2BEB-4C19-99F9-9FC3C46725F3}">
+    <comment ref="AL1" authorId="0" shapeId="0" xr:uid="{28DEFE86-2BEB-4C19-99F9-9FC3C46725F3}">
       <text>
         <r>
           <rPr>
@@ -408,7 +514,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH1" authorId="0" shapeId="0" xr:uid="{9189F978-0462-4031-826A-0220C3A0FBE8}">
+    <comment ref="AM1" authorId="0" shapeId="0" xr:uid="{9189F978-0462-4031-826A-0220C3A0FBE8}">
       <text>
         <r>
           <rPr>
@@ -432,7 +538,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ1" authorId="0" shapeId="0" xr:uid="{C19C0D7F-4226-4736-BA35-E6E08EBBAC7A}">
+    <comment ref="AO1" authorId="0" shapeId="0" xr:uid="{C19C0D7F-4226-4736-BA35-E6E08EBBAC7A}">
       <text>
         <r>
           <rPr>
@@ -456,7 +562,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK1" authorId="0" shapeId="0" xr:uid="{AB0FF933-2837-4C7D-A183-D59581906014}">
+    <comment ref="AP1" authorId="0" shapeId="0" xr:uid="{AB0FF933-2837-4C7D-A183-D59581906014}">
       <text>
         <r>
           <rPr>
@@ -480,7 +586,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL1" authorId="0" shapeId="0" xr:uid="{783213B1-12E4-4FD7-BD87-ED5859C4959C}">
+    <comment ref="AQ1" authorId="0" shapeId="0" xr:uid="{783213B1-12E4-4FD7-BD87-ED5859C4959C}">
       <text>
         <r>
           <rPr>
@@ -509,7 +615,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="181">
   <si>
     <t>&lt;/jt:forEach&gt;</t>
   </si>
@@ -863,12 +969,6 @@
   </si>
   <si>
     <t>MARI</t>
-  </si>
-  <si>
-    <t>BAFA GENERAL</t>
-  </si>
-  <si>
-    <t>BAFD GENERAL</t>
   </si>
   <si>
     <t>BAFD PERFECTIONNEMENT</t>
@@ -1020,13 +1120,67 @@
   </si>
   <si>
     <t>$[V4-U4]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPRO ANIM </t>
+  </si>
+  <si>
+    <t>${chef.formation.appro_anim.datefin}</t>
+  </si>
+  <si>
+    <t>${chef.formation.appro_accueil.datefin}</t>
+  </si>
+  <si>
+    <t>APPRO ANIM</t>
+  </si>
+  <si>
+    <t>${unite.appro_anim}</t>
+  </si>
+  <si>
+    <t>${unite.appro_accueil}</t>
+  </si>
+  <si>
+    <t>${chef.formation.module_appro_accueil_scoutisme.datefin}</t>
+  </si>
+  <si>
+    <t>MODULE APPRO ACCUEIL DE SCOUTISME</t>
+  </si>
+  <si>
+    <t>${chef.formation.module_animateur_scoutisme_campisme.datefin}</t>
+  </si>
+  <si>
+    <t>${chef.formation.module_appro_surveillant_baignade.datefin}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MODULE ANIMATEUR DE SCOUTISME ET CAMPISME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPRO SURVEILLANT DE BAIGNADE </t>
+  </si>
+  <si>
+    <t>${unite.module_appro_accueil_scoutisme}</t>
+  </si>
+  <si>
+    <t>${unite.module_animateur_scoutisme_campisme}</t>
+  </si>
+  <si>
+    <t>${unite.module_appro_surveillant_baignade}</t>
+  </si>
+  <si>
+    <t>APPRO ACCUEIL DE SCOUTISME</t>
+  </si>
+  <si>
+    <t>BAFA FORMATION GÉNÉRALE</t>
+  </si>
+  <si>
+    <t>BAFD FORMATION GÉNÉRALE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1110,6 +1264,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1827,6 +1994,12 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Sébastien Bouchex" id="{D2D877DA-17D9-4BDD-B14D-4E2D1B208222}" userId="S::sbouchex@infovista.com::4b272613-d5ab-4e32-92d1-b65864253ecd" providerId="AD"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
@@ -2127,13 +2300,13 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:AL3"/>
+  <dimension ref="A1:AQ3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2152,17 +2325,22 @@
     <col min="15" max="15" width="2.5703125" style="18" customWidth="1"/>
     <col min="16" max="16" width="14.7109375" style="18" customWidth="1"/>
     <col min="17" max="17" width="2.85546875" style="2" customWidth="1"/>
-    <col min="18" max="25" width="11.42578125" style="38" customWidth="1"/>
-    <col min="26" max="26" width="17.5703125" style="38" customWidth="1"/>
-    <col min="27" max="27" width="3.140625" style="2" customWidth="1"/>
-    <col min="28" max="34" width="11.42578125" style="38" customWidth="1"/>
-    <col min="35" max="35" width="11.42578125" style="18" customWidth="1"/>
-    <col min="36" max="36" width="12.7109375" style="2" customWidth="1"/>
-    <col min="37" max="37" width="15" style="18" customWidth="1"/>
-    <col min="38" max="38" width="14.140625" style="18" customWidth="1"/>
+    <col min="18" max="20" width="11.42578125" style="38" customWidth="1"/>
+    <col min="21" max="21" width="12.42578125" style="38" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" style="38" customWidth="1"/>
+    <col min="23" max="23" width="14.140625" style="38" customWidth="1"/>
+    <col min="24" max="25" width="13" style="38" customWidth="1"/>
+    <col min="26" max="30" width="11.42578125" style="38" customWidth="1"/>
+    <col min="31" max="31" width="17.5703125" style="38" customWidth="1"/>
+    <col min="32" max="32" width="3.140625" style="2" customWidth="1"/>
+    <col min="33" max="39" width="11.42578125" style="38" customWidth="1"/>
+    <col min="40" max="40" width="4" style="18" customWidth="1"/>
+    <col min="41" max="41" width="12.7109375" style="2" customWidth="1"/>
+    <col min="42" max="42" width="15" style="18" customWidth="1"/>
+    <col min="43" max="43" width="14.140625" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="30" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:43" s="30" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>3</v>
       </c>
@@ -2224,61 +2402,76 @@
         <v>10</v>
       </c>
       <c r="U1" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="V1" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="W1" s="39" t="s">
+        <v>170</v>
+      </c>
+      <c r="X1" s="39" t="s">
+        <v>173</v>
+      </c>
+      <c r="Y1" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="Z1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="39" t="s">
+      <c r="AA1" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="W1" s="39" t="s">
+      <c r="AB1" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="X1" s="39" t="s">
+      <c r="AC1" s="39" t="s">
+        <v>179</v>
+      </c>
+      <c r="AD1" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="AE1" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="Y1" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="Z1" s="39" t="s">
-        <v>119</v>
-      </c>
-      <c r="AA1" s="31" t="s">
+      <c r="AF1" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="AB1" s="40" t="s">
+      <c r="AG1" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="AC1" s="40" t="s">
+      <c r="AH1" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="40" t="s">
+      <c r="AI1" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="AE1" s="40" t="s">
+      <c r="AJ1" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="AF1" s="40" t="s">
+      <c r="AK1" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="AG1" s="40" t="s">
+      <c r="AL1" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="AH1" s="40" t="s">
+      <c r="AM1" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="AI1" s="31" t="s">
+      <c r="AN1" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="AJ1" s="22" t="s">
+      <c r="AO1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="AK1" s="25" t="s">
+      <c r="AP1" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="AL1" s="25" t="s">
+      <c r="AQ1" s="25" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>83</v>
       </c>
@@ -2333,57 +2526,72 @@
         <v>46</v>
       </c>
       <c r="U2" s="38" t="s">
+        <v>165</v>
+      </c>
+      <c r="V2" s="38" t="s">
+        <v>164</v>
+      </c>
+      <c r="W2" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="X2" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="Y2" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z2" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="V2" s="38" t="s">
+      <c r="AA2" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="W2" s="38" t="s">
+      <c r="AB2" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="AC2" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="AD2" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="X2" s="38" t="s">
+      <c r="AE2" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="Y2" s="38" t="s">
-        <v>122</v>
-      </c>
-      <c r="Z2" s="38" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA2" s="10"/>
-      <c r="AB2" s="38" t="s">
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="AC2" s="38" t="s">
+      <c r="AH2" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="AD2" s="38" t="s">
+      <c r="AI2" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="AE2" s="38" t="s">
+      <c r="AJ2" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="AF2" s="38" t="s">
+      <c r="AK2" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="AG2" s="38" t="s">
+      <c r="AL2" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="AH2" s="38" t="s">
+      <c r="AM2" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="AI2" s="3"/>
-      <c r="AJ2" s="36" t="s">
+      <c r="AN2" s="3"/>
+      <c r="AO2" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AP2" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="AL2" s="3" t="s">
-        <v>129</v>
+      <c r="AQ2" s="3" t="s">
+        <v>127</v>
       </c>
     </row>
-    <row r="3" spans="1:38" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>87</v>
       </c>
@@ -2438,64 +2646,79 @@
         <v>46</v>
       </c>
       <c r="U3" s="38" t="s">
+        <v>165</v>
+      </c>
+      <c r="V3" s="38" t="s">
+        <v>164</v>
+      </c>
+      <c r="W3" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="X3" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="Y3" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z3" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="V3" s="38" t="s">
+      <c r="AA3" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="W3" s="38" t="s">
+      <c r="AB3" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="AC3" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="AD3" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="X3" s="38" t="s">
+      <c r="AE3" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="Y3" s="38" t="s">
-        <v>122</v>
-      </c>
-      <c r="Z3" s="38" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA3" s="10"/>
-      <c r="AB3" s="38" t="s">
+      <c r="AF3" s="10"/>
+      <c r="AG3" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="AC3" s="38" t="s">
+      <c r="AH3" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="AD3" s="38" t="s">
+      <c r="AI3" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="AE3" s="38" t="s">
+      <c r="AJ3" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="AF3" s="38" t="s">
+      <c r="AK3" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="AG3" s="38" t="s">
+      <c r="AL3" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="AH3" s="38" t="s">
+      <c r="AM3" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="AI3" s="3"/>
-      <c r="AJ3" s="36" t="s">
+      <c r="AN3" s="3"/>
+      <c r="AO3" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="AK3" s="3" t="s">
+      <c r="AP3" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="AL3" s="3" t="s">
-        <v>129</v>
+      <c r="AQ3" s="3" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AL3" xr:uid="{D6BF73C0-3DFA-4EF7-83FF-A6F179361B6B}"/>
-  <conditionalFormatting sqref="AL2:AL65536">
+  <autoFilter ref="A1:AQ3" xr:uid="{D6BF73C0-3DFA-4EF7-83FF-A6F179361B6B}"/>
+  <conditionalFormatting sqref="AQ2:AQ65536">
     <cfRule type="cellIs" dxfId="30" priority="24" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK2:AK65536">
+  <conditionalFormatting sqref="AP2:AP65536">
     <cfRule type="cellIs" dxfId="29" priority="14" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
@@ -2543,13 +2766,13 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:X4"/>
+  <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2557,15 +2780,25 @@
     <col min="1" max="1" width="75.28515625" style="9" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" style="13" customWidth="1"/>
     <col min="3" max="3" width="18.140625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="18" customWidth="1"/>
+    <col min="4" max="4" width="3.7109375" style="18" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="2"/>
     <col min="6" max="7" width="8.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="18" customWidth="1"/>
-    <col min="9" max="15" width="8.85546875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="10.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="3.42578125" style="18" customWidth="1"/>
+    <col min="9" max="10" width="8.85546875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="3.140625" style="18" customWidth="1"/>
+    <col min="12" max="13" width="8.85546875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="18" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="18" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="15.28515625" style="18" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" style="18" customWidth="1"/>
+    <col min="19" max="19" width="13.5703125" style="18" customWidth="1"/>
+    <col min="20" max="20" width="3.140625" style="18" customWidth="1"/>
+    <col min="21" max="22" width="8.85546875" style="2" customWidth="1"/>
+    <col min="23" max="23" width="10.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" s="30" customFormat="1" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>18</v>
       </c>
@@ -2596,32 +2829,53 @@
       <c r="J1" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="28" t="s">
+      <c r="K1" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="28" t="s">
+      <c r="M1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="28" t="s">
+      <c r="N1" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="29" t="s">
+      <c r="O1" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="P1" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q1" s="39" t="s">
+        <v>170</v>
+      </c>
+      <c r="R1" s="39" t="s">
+        <v>173</v>
+      </c>
+      <c r="S1" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="T1" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="U1" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="29" t="s">
+      <c r="V1" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="29" t="s">
+      <c r="W1" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="29" t="s">
+      <c r="X1" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="29" t="s">
+      <c r="Y1" s="29" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>64</v>
       </c>
@@ -2648,42 +2902,63 @@
       <c r="J2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="10"/>
+      <c r="L2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q2" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="R2" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="S2" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="T2" s="10"/>
+      <c r="U2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="X2" s="1" t="s">
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AE2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="R4" s="1"/>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="K3" s="10"/>
+      <c r="T3" s="10"/>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="Y4" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R2" xr:uid="{28350664-D0B6-4E87-AB67-D67C35BD65E8}"/>
+  <autoFilter ref="A1:Y2" xr:uid="{28350664-D0B6-4E87-AB67-D67C35BD65E8}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2741,7 +3016,7 @@
       <c r="D1" s="45"/>
       <c r="E1" s="45"/>
       <c r="F1" s="25" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G1" s="25" t="s">
         <v>115</v>
@@ -2773,12 +3048,12 @@
       <c r="R1" s="77"/>
       <c r="S1" s="46"/>
       <c r="T1" s="73" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="U1" s="76"/>
       <c r="V1" s="77"/>
       <c r="W1" s="76" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="X1" s="76"/>
       <c r="Y1" s="77"/>
@@ -2833,7 +3108,7 @@
         <v>99</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G3" s="25" t="s">
         <v>101</v>
@@ -2907,7 +3182,7 @@
     </row>
     <row r="4" spans="1:29" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C4" s="44"/>
       <c r="D4" s="8" t="s">
@@ -2917,58 +3192,58 @@
         <v>58</v>
       </c>
       <c r="F4" s="49" t="s">
+        <v>133</v>
+      </c>
+      <c r="G4" s="49" t="s">
+        <v>134</v>
+      </c>
+      <c r="H4" s="49" t="s">
         <v>135</v>
       </c>
-      <c r="G4" s="49" t="s">
+      <c r="I4" s="49" t="s">
         <v>136</v>
       </c>
-      <c r="H4" s="49" t="s">
+      <c r="J4" s="49" t="s">
         <v>137</v>
-      </c>
-      <c r="I4" s="49" t="s">
-        <v>138</v>
-      </c>
-      <c r="J4" s="49" t="s">
-        <v>139</v>
       </c>
       <c r="K4" s="50"/>
       <c r="L4" s="51">
         <v>1</v>
       </c>
       <c r="M4" s="53" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="N4" s="49" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="O4" s="51"/>
       <c r="P4" s="51" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="Q4" s="51" t="s">
         <v>107</v>
       </c>
       <c r="R4" s="51" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="S4" s="51"/>
       <c r="T4" s="51" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="U4" s="8" t="s">
         <v>109</v>
       </c>
       <c r="V4" s="49" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="W4" s="51" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="X4" s="8" t="s">
         <v>110</v>
       </c>
       <c r="Y4" s="49" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="Z4" s="52"/>
       <c r="AA4" s="51">
@@ -2978,7 +3253,7 @@
         <v>108</v>
       </c>
       <c r="AC4" s="49" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:29" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -3114,16 +3389,16 @@
       <c r="E1" s="81"/>
       <c r="F1" s="18"/>
       <c r="G1" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="H1" s="25" t="s">
-        <v>159</v>
-      </c>
       <c r="I1" s="25" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J1" s="25" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K1" s="25" t="s">
         <v>27</v>
@@ -3140,19 +3415,19 @@
         <v>78</v>
       </c>
       <c r="Q1" s="73" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="R1" s="76"/>
       <c r="S1" s="77"/>
       <c r="T1" s="46"/>
       <c r="U1" s="73" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="V1" s="76"/>
       <c r="W1" s="77"/>
       <c r="X1" s="68"/>
       <c r="Y1" s="73" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="Z1" s="76"/>
       <c r="AA1" s="77"/>
@@ -3311,32 +3586,32 @@
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="J4" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="K4" s="8" t="s">
         <v>150</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>152</v>
       </c>
       <c r="L4" s="50"/>
       <c r="M4" s="57" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N4" s="58" t="s">
         <v>33</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Q4" s="51" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="R4" s="57" t="s">
         <v>107</v>
@@ -3345,19 +3620,19 @@
         <v>106</v>
       </c>
       <c r="U4" s="51" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="V4" s="51" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="Y4" s="51" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="Z4" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="AA4" s="8" t="s">
         <v>105</v>
@@ -3369,7 +3644,7 @@
         <v>111</v>
       </c>
       <c r="AE4" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3492,7 +3767,7 @@
         <v>37</v>
       </c>
       <c r="B1" s="35">
-        <v>43481</v>
+        <v>43489</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Correction APF et RG
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele.xlsx
+++ b/fichiers/conf/modele.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2D84A9-A98F-4E49-AB4D-9B330BBFB84A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66537B2-F4B6-4ECF-A7E4-18C3839065D5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="477" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="2055" yWindow="255" windowWidth="26160" windowHeight="13935" tabRatio="477" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Responsables" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,10 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Quotas Année'!$A$3:$AC$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Quotas Camps'!$A$3:$AE$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Responsables!$A$1:$AQ$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Synthèse par unité'!$A$1:$Y$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Responsables!$A$1:$AW$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Synthèse par unité'!$A$1:$AE$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -168,7 +168,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{55CC420A-73E2-4858-9D36-083E75638385}">
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{BD73F079-BD47-4A9B-9DB9-888F403257F2}">
       <text>
         <r>
           <rPr>
@@ -176,7 +176,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>Sébastien:</t>
         </r>
@@ -185,14 +185,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 Fin de stage</t>
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{E842F17D-4EA4-46A7-8AA9-D11373D8D411}">
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{4EEDDAC8-2343-467D-9346-63590EC6F6AE}">
       <text>
         <r>
           <rPr>
@@ -200,7 +200,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>Sébastien:</t>
         </r>
@@ -209,14 +209,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 Fin de stage</t>
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{83C77407-EDE7-4503-93FD-393628AE54E4}">
+    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{6A99CB9E-35A8-4FA1-BC9B-4D96C495F872}">
       <text>
         <r>
           <rPr>
@@ -224,7 +224,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>Sébastien:</t>
         </r>
@@ -233,14 +233,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 Fin de stage</t>
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{83CCAF6B-404B-4C1D-92E5-BE497427DD7D}">
+    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{86FD4D1A-31E9-4CF5-B839-4DB3C6578C7B}">
       <text>
         <r>
           <rPr>
@@ -248,7 +248,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>Sébastien:</t>
         </r>
@@ -257,14 +257,134 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 Fin de stage</t>
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{156BCBB7-1FAF-413C-8ECC-A4A9CA20E3FD}">
+    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{D4CB2E41-2D86-492F-A896-A7F2621165D9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sébastien:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Fin de stage</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{55CC420A-73E2-4858-9D36-083E75638385}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sébastien:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fin de stage</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{E842F17D-4EA4-46A7-8AA9-D11373D8D411}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sébastien:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fin de stage</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{83C77407-EDE7-4503-93FD-393628AE54E4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sébastien:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fin de stage</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{83CCAF6B-404B-4C1D-92E5-BE497427DD7D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sébastien:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fin de stage</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AD1" authorId="0" shapeId="0" xr:uid="{156BCBB7-1FAF-413C-8ECC-A4A9CA20E3FD}">
       <text>
         <r>
           <rPr>
@@ -298,7 +418,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{2C5F74EA-D518-4557-AC0F-8BFFC404907C}">
+    <comment ref="AE1" authorId="0" shapeId="0" xr:uid="{2C5F74EA-D518-4557-AC0F-8BFFC404907C}">
       <text>
         <r>
           <rPr>
@@ -322,7 +442,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{6045E9B0-AA1D-41B4-9C3C-BC746D9BC589}">
+    <comment ref="AF1" authorId="0" shapeId="0" xr:uid="{6045E9B0-AA1D-41B4-9C3C-BC746D9BC589}">
       <text>
         <r>
           <rPr>
@@ -346,7 +466,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{1F3E1ACB-E2A6-4A98-A36E-7ABE327D55F6}">
+    <comment ref="AG1" authorId="0" shapeId="0" xr:uid="{1F3E1ACB-E2A6-4A98-A36E-7ABE327D55F6}">
       <text>
         <r>
           <rPr>
@@ -370,7 +490,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG1" authorId="0" shapeId="0" xr:uid="{D7CCADB1-4D8A-4BC8-905C-D1BA438E77F1}">
+    <comment ref="AM1" authorId="0" shapeId="0" xr:uid="{D7CCADB1-4D8A-4BC8-905C-D1BA438E77F1}">
       <text>
         <r>
           <rPr>
@@ -394,7 +514,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH1" authorId="0" shapeId="0" xr:uid="{E9756D3C-D426-47A5-A95D-19409772C521}">
+    <comment ref="AN1" authorId="0" shapeId="0" xr:uid="{E9756D3C-D426-47A5-A95D-19409772C521}">
       <text>
         <r>
           <rPr>
@@ -418,7 +538,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI1" authorId="0" shapeId="0" xr:uid="{2F31B678-BEA5-4DB4-AC1D-AC1EC879D750}">
+    <comment ref="AO1" authorId="0" shapeId="0" xr:uid="{2F31B678-BEA5-4DB4-AC1D-AC1EC879D750}">
       <text>
         <r>
           <rPr>
@@ -442,7 +562,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ1" authorId="0" shapeId="0" xr:uid="{C8A48C2F-9EB4-4B10-8DBC-DE0A2B010CD5}">
+    <comment ref="AP1" authorId="0" shapeId="0" xr:uid="{C8A48C2F-9EB4-4B10-8DBC-DE0A2B010CD5}">
       <text>
         <r>
           <rPr>
@@ -466,7 +586,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK1" authorId="0" shapeId="0" xr:uid="{CE08BEFE-EAC8-4844-983C-8BADEFBFE2C5}">
+    <comment ref="AQ1" authorId="0" shapeId="0" xr:uid="{CE08BEFE-EAC8-4844-983C-8BADEFBFE2C5}">
       <text>
         <r>
           <rPr>
@@ -490,7 +610,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL1" authorId="0" shapeId="0" xr:uid="{28DEFE86-2BEB-4C19-99F9-9FC3C46725F3}">
+    <comment ref="AR1" authorId="0" shapeId="0" xr:uid="{28DEFE86-2BEB-4C19-99F9-9FC3C46725F3}">
       <text>
         <r>
           <rPr>
@@ -514,7 +634,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM1" authorId="0" shapeId="0" xr:uid="{9189F978-0462-4031-826A-0220C3A0FBE8}">
+    <comment ref="AS1" authorId="0" shapeId="0" xr:uid="{9189F978-0462-4031-826A-0220C3A0FBE8}">
       <text>
         <r>
           <rPr>
@@ -538,7 +658,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO1" authorId="0" shapeId="0" xr:uid="{C19C0D7F-4226-4736-BA35-E6E08EBBAC7A}">
+    <comment ref="AU1" authorId="0" shapeId="0" xr:uid="{C19C0D7F-4226-4736-BA35-E6E08EBBAC7A}">
       <text>
         <r>
           <rPr>
@@ -562,7 +682,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP1" authorId="0" shapeId="0" xr:uid="{AB0FF933-2837-4C7D-A183-D59581906014}">
+    <comment ref="AV1" authorId="0" shapeId="0" xr:uid="{AB0FF933-2837-4C7D-A183-D59581906014}">
       <text>
         <r>
           <rPr>
@@ -586,7 +706,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ1" authorId="0" shapeId="0" xr:uid="{783213B1-12E4-4FD7-BD87-ED5859C4959C}">
+    <comment ref="AW1" authorId="0" shapeId="0" xr:uid="{783213B1-12E4-4FD7-BD87-ED5859C4959C}">
       <text>
         <r>
           <rPr>
@@ -615,7 +735,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="194">
   <si>
     <t>&lt;/jt:forEach&gt;</t>
   </si>
@@ -747,9 +867,6 @@
   </si>
   <si>
     <t>&lt;jt:if test="${unite.avecdesjeunes}"&gt;${unite.ratio}&lt;/jt:if&gt;</t>
-  </si>
-  <si>
-    <t>${chef.formation.apf.datefin}</t>
   </si>
   <si>
     <t>${chef.formation.tech.datefin}</t>
@@ -1174,6 +1291,48 @@
   </si>
   <si>
     <t>BAFD FORMATION GÉNÉRALE</t>
+  </si>
+  <si>
+    <t>APF CHEFS-CHEFTAINES</t>
+  </si>
+  <si>
+    <t>APF RESPONSABLES de GROUPE</t>
+  </si>
+  <si>
+    <t>AIDE A LA PRISE DE FONCTION</t>
+  </si>
+  <si>
+    <t>${chef.formation.apf.datefin}</t>
+  </si>
+  <si>
+    <t>${chef.formation.apf_chefs.datefin}</t>
+  </si>
+  <si>
+    <t>${chef.formation.apf_rg.datefin}</t>
+  </si>
+  <si>
+    <t>APF SECRETAIRE TRESORIER</t>
+  </si>
+  <si>
+    <t>APF AUMONIER ET AVSC</t>
+  </si>
+  <si>
+    <t>${chef.formation.apf_sp.datefin}</t>
+  </si>
+  <si>
+    <t>${chef.formation.apf_aavsc.datefin}</t>
+  </si>
+  <si>
+    <t>APF RESPONSABLE LOCAL DEVELOPPEMENT ET RESEAUX</t>
+  </si>
+  <si>
+    <t>${chef.formation.apf_rldr.datefin}</t>
+  </si>
+  <si>
+    <t>FORMATION ACCUEIL DE SCOUTISME RG</t>
+  </si>
+  <si>
+    <t>${chef.formation.accueil_scoutisme_rg.datefin}</t>
   </si>
 </sst>
 </file>
@@ -2300,13 +2459,13 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:AQ3"/>
+  <dimension ref="A1:AW3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y1" sqref="Y1"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2325,22 +2484,28 @@
     <col min="15" max="15" width="2.5703125" style="18" customWidth="1"/>
     <col min="16" max="16" width="14.7109375" style="18" customWidth="1"/>
     <col min="17" max="17" width="2.85546875" style="2" customWidth="1"/>
-    <col min="18" max="20" width="11.42578125" style="38" customWidth="1"/>
-    <col min="21" max="21" width="12.42578125" style="38" customWidth="1"/>
-    <col min="22" max="22" width="11.42578125" style="38" customWidth="1"/>
-    <col min="23" max="23" width="14.140625" style="38" customWidth="1"/>
-    <col min="24" max="25" width="13" style="38" customWidth="1"/>
-    <col min="26" max="30" width="11.42578125" style="38" customWidth="1"/>
-    <col min="31" max="31" width="17.5703125" style="38" customWidth="1"/>
-    <col min="32" max="32" width="3.140625" style="2" customWidth="1"/>
-    <col min="33" max="39" width="11.42578125" style="38" customWidth="1"/>
-    <col min="40" max="40" width="4" style="18" customWidth="1"/>
-    <col min="41" max="41" width="12.7109375" style="2" customWidth="1"/>
-    <col min="42" max="42" width="15" style="18" customWidth="1"/>
-    <col min="43" max="43" width="14.140625" style="18" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="38" customWidth="1"/>
+    <col min="19" max="19" width="11.140625" style="38" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" style="38" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="38" customWidth="1"/>
+    <col min="22" max="22" width="18" style="38" customWidth="1"/>
+    <col min="23" max="24" width="14.28515625" style="38" customWidth="1"/>
+    <col min="25" max="26" width="11.42578125" style="38" customWidth="1"/>
+    <col min="27" max="27" width="12.42578125" style="38" customWidth="1"/>
+    <col min="28" max="28" width="11.42578125" style="38" customWidth="1"/>
+    <col min="29" max="29" width="14.140625" style="38" customWidth="1"/>
+    <col min="30" max="31" width="13" style="38" customWidth="1"/>
+    <col min="32" max="36" width="11.42578125" style="38" customWidth="1"/>
+    <col min="37" max="37" width="17.5703125" style="38" customWidth="1"/>
+    <col min="38" max="38" width="3.140625" style="2" customWidth="1"/>
+    <col min="39" max="45" width="11.42578125" style="38" customWidth="1"/>
+    <col min="46" max="46" width="4" style="18" customWidth="1"/>
+    <col min="47" max="47" width="12.7109375" style="2" customWidth="1"/>
+    <col min="48" max="48" width="15" style="18" customWidth="1"/>
+    <col min="49" max="49" width="14.140625" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="30" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:49" s="30" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>3</v>
       </c>
@@ -2354,126 +2519,144 @@
         <v>18</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H1" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="J1" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="K1" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="L1" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="L1" s="37" t="s">
+      <c r="M1" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="N1" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="O1" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="P1" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q1" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="R1" s="39" t="s">
+        <v>182</v>
+      </c>
+      <c r="S1" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="T1" s="39" t="s">
+        <v>181</v>
+      </c>
+      <c r="U1" s="39" t="s">
+        <v>186</v>
+      </c>
+      <c r="V1" s="39" t="s">
+        <v>190</v>
+      </c>
+      <c r="W1" s="39" t="s">
+        <v>187</v>
+      </c>
+      <c r="X1" s="39" t="s">
+        <v>192</v>
+      </c>
+      <c r="Y1" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z1" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA1" s="39" t="s">
+        <v>177</v>
+      </c>
+      <c r="AB1" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="AC1" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD1" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="AE1" s="39" t="s">
+        <v>173</v>
+      </c>
+      <c r="AF1" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG1" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH1" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="AI1" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="AJ1" s="39" t="s">
+        <v>179</v>
+      </c>
+      <c r="AK1" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="AL1" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM1" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="AN1" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="AO1" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="AP1" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="AQ1" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="AR1" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="AS1" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="AT1" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="AU1" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="AV1" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="AW1" s="25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
         <v>82</v>
-      </c>
-      <c r="M1" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="N1" s="41" t="s">
-        <v>92</v>
-      </c>
-      <c r="O1" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="P1" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q1" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="R1" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="S1" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="T1" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="U1" s="39" t="s">
-        <v>178</v>
-      </c>
-      <c r="V1" s="39" t="s">
-        <v>163</v>
-      </c>
-      <c r="W1" s="39" t="s">
-        <v>170</v>
-      </c>
-      <c r="X1" s="39" t="s">
-        <v>173</v>
-      </c>
-      <c r="Y1" s="39" t="s">
-        <v>174</v>
-      </c>
-      <c r="Z1" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA1" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB1" s="39" t="s">
-        <v>116</v>
-      </c>
-      <c r="AC1" s="39" t="s">
-        <v>179</v>
-      </c>
-      <c r="AD1" s="39" t="s">
-        <v>180</v>
-      </c>
-      <c r="AE1" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="AF1" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="AG1" s="40" t="s">
-        <v>13</v>
-      </c>
-      <c r="AH1" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="AI1" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="AJ1" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="AK1" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="AL1" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="AM1" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="AN1" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="AO1" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="AP1" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="AQ1" s="25" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
-        <v>83</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -2482,118 +2665,136 @@
         <v>2</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I2" s="38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J2" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K2" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="L2" s="38" t="s">
-        <v>61</v>
-      </c>
       <c r="M2" s="42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N2" s="42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O2" s="10"/>
       <c r="P2" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q2" s="10"/>
       <c r="R2" s="38" t="s">
+        <v>183</v>
+      </c>
+      <c r="S2" s="38" t="s">
+        <v>184</v>
+      </c>
+      <c r="T2" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="U2" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="V2" s="38" t="s">
+        <v>191</v>
+      </c>
+      <c r="W2" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="X2" s="38" t="s">
+        <v>193</v>
+      </c>
+      <c r="Y2" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="S2" s="38" t="s">
+      <c r="Z2" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="T2" s="38" t="s">
+      <c r="AA2" s="38" t="s">
+        <v>164</v>
+      </c>
+      <c r="AB2" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="AC2" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="AD2" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="AE2" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="AF2" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="U2" s="38" t="s">
-        <v>165</v>
-      </c>
-      <c r="V2" s="38" t="s">
-        <v>164</v>
-      </c>
-      <c r="W2" s="38" t="s">
-        <v>169</v>
-      </c>
-      <c r="X2" s="38" t="s">
-        <v>171</v>
-      </c>
-      <c r="Y2" s="38" t="s">
-        <v>172</v>
-      </c>
-      <c r="Z2" s="38" t="s">
+      <c r="AG2" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="AA2" s="38" t="s">
+      <c r="AH2" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI2" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ2" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="AK2" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL2" s="10"/>
+      <c r="AM2" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="AB2" s="38" t="s">
-        <v>118</v>
-      </c>
-      <c r="AC2" s="38" t="s">
-        <v>119</v>
-      </c>
-      <c r="AD2" s="38" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE2" s="38" t="s">
-        <v>121</v>
-      </c>
-      <c r="AF2" s="10"/>
-      <c r="AG2" s="38" t="s">
+      <c r="AN2" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="AH2" s="38" t="s">
+      <c r="AO2" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="AI2" s="38" t="s">
+      <c r="AP2" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="AJ2" s="38" t="s">
+      <c r="AQ2" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR2" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="AK2" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="AL2" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="AM2" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="AN2" s="3"/>
-      <c r="AO2" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="AP2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="AQ2" s="3" t="s">
-        <v>127</v>
+      <c r="AS2" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="AT2" s="3"/>
+      <c r="AU2" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="AV2" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AW2" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:43" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:49" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>1</v>
@@ -2602,123 +2803,141 @@
         <v>2</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I3" s="38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J3" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K3" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="L3" s="38" t="s">
-        <v>61</v>
-      </c>
       <c r="M3" s="42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N3" s="42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O3" s="10"/>
       <c r="P3" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q3" s="10"/>
       <c r="R3" s="38" t="s">
+        <v>183</v>
+      </c>
+      <c r="S3" s="38" t="s">
+        <v>184</v>
+      </c>
+      <c r="T3" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="U3" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="V3" s="38" t="s">
+        <v>191</v>
+      </c>
+      <c r="W3" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="X3" s="38" t="s">
+        <v>193</v>
+      </c>
+      <c r="Y3" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="S3" s="38" t="s">
+      <c r="Z3" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="T3" s="38" t="s">
+      <c r="AA3" s="38" t="s">
+        <v>164</v>
+      </c>
+      <c r="AB3" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="AC3" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="AD3" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="AE3" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="AF3" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="U3" s="38" t="s">
-        <v>165</v>
-      </c>
-      <c r="V3" s="38" t="s">
-        <v>164</v>
-      </c>
-      <c r="W3" s="38" t="s">
-        <v>169</v>
-      </c>
-      <c r="X3" s="38" t="s">
-        <v>171</v>
-      </c>
-      <c r="Y3" s="38" t="s">
-        <v>172</v>
-      </c>
-      <c r="Z3" s="38" t="s">
+      <c r="AG3" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="AA3" s="38" t="s">
+      <c r="AH3" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI3" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ3" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="AK3" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL3" s="10"/>
+      <c r="AM3" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="AB3" s="38" t="s">
-        <v>118</v>
-      </c>
-      <c r="AC3" s="38" t="s">
-        <v>119</v>
-      </c>
-      <c r="AD3" s="38" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE3" s="38" t="s">
-        <v>121</v>
-      </c>
-      <c r="AF3" s="10"/>
-      <c r="AG3" s="38" t="s">
+      <c r="AN3" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="AH3" s="38" t="s">
+      <c r="AO3" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="AI3" s="38" t="s">
+      <c r="AP3" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="AJ3" s="38" t="s">
+      <c r="AQ3" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR3" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="AK3" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="AL3" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="AM3" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="AN3" s="3"/>
-      <c r="AO3" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="AP3" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="AQ3" s="3" t="s">
-        <v>127</v>
+      <c r="AS3" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="AT3" s="3"/>
+      <c r="AU3" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="AV3" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AW3" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AQ3" xr:uid="{D6BF73C0-3DFA-4EF7-83FF-A6F179361B6B}"/>
-  <conditionalFormatting sqref="AQ2:AQ65536">
+  <autoFilter ref="A1:AW3" xr:uid="{D6BF73C0-3DFA-4EF7-83FF-A6F179361B6B}"/>
+  <conditionalFormatting sqref="AW2:AW65536">
     <cfRule type="cellIs" dxfId="30" priority="24" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AP2:AP65536">
+  <conditionalFormatting sqref="AV2:AV65536">
     <cfRule type="cellIs" dxfId="29" priority="14" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
@@ -2786,16 +3005,14 @@
     <col min="8" max="8" width="3.42578125" style="18" customWidth="1"/>
     <col min="9" max="10" width="8.85546875" style="2" customWidth="1"/>
     <col min="11" max="11" width="3.140625" style="18" customWidth="1"/>
-    <col min="12" max="13" width="8.85546875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="18" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" style="18" customWidth="1"/>
-    <col min="16" max="16" width="8.85546875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="15.28515625" style="18" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" style="18" customWidth="1"/>
-    <col min="19" max="19" width="13.5703125" style="18" customWidth="1"/>
-    <col min="20" max="20" width="3.140625" style="18" customWidth="1"/>
-    <col min="21" max="22" width="8.85546875" style="2" customWidth="1"/>
-    <col min="23" max="23" width="10.42578125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="5" style="2" customWidth="1"/>
+    <col min="13" max="13" width="5.5703125" style="18" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" customWidth="1"/>
+    <col min="18" max="18" width="17.28515625" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" s="30" customFormat="1" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2803,13 +3020,13 @@
         <v>18</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D1" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E1" s="22" t="s">
         <v>19</v>
@@ -2821,7 +3038,7 @@
         <v>21</v>
       </c>
       <c r="H1" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I1" s="26" t="s">
         <v>23</v>
@@ -2830,9 +3047,9 @@
         <v>22</v>
       </c>
       <c r="K1" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="L1" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="L1" s="39" t="s">
         <v>8</v>
       </c>
       <c r="M1" s="28" t="s">
@@ -2842,22 +3059,22 @@
         <v>10</v>
       </c>
       <c r="O1" s="28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="P1" s="28" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q1" s="39" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="R1" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="S1" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="S1" s="39" t="s">
-        <v>174</v>
-      </c>
       <c r="T1" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="U1" s="29" t="s">
         <v>27</v>
@@ -2877,13 +3094,13 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="4" t="s">
@@ -2900,10 +3117,10 @@
         <v>33</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K2" s="10"/>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="18" t="s">
         <v>28</v>
       </c>
       <c r="M2" s="2" t="s">
@@ -2913,19 +3130,19 @@
         <v>30</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q2" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="R2" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="R2" s="18" t="s">
+      <c r="S2" s="18" t="s">
         <v>176</v>
-      </c>
-      <c r="S2" s="18" t="s">
-        <v>177</v>
       </c>
       <c r="T2" s="10"/>
       <c r="U2" s="2" t="s">
@@ -2952,13 +3169,13 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="K3" s="10"/>
-      <c r="T3" s="10"/>
+      <c r="M3" s="10"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="Y4" s="1"/>
+      <c r="R4" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Y2" xr:uid="{28350664-D0B6-4E87-AB67-D67C35BD65E8}"/>
+  <autoFilter ref="A1:AE1" xr:uid="{66A8F9AA-9955-4F38-8C09-E2219E483C8B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3016,49 +3233,49 @@
       <c r="D1" s="45"/>
       <c r="E1" s="45"/>
       <c r="F1" s="25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G1" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H1" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" s="25" t="s">
         <v>113</v>
-      </c>
-      <c r="I1" s="25" t="s">
-        <v>114</v>
       </c>
       <c r="J1" s="25" t="s">
         <v>27</v>
       </c>
       <c r="K1" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L1" s="73" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M1" s="74"/>
       <c r="N1" s="75"/>
       <c r="O1" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P1" s="73" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q1" s="76"/>
       <c r="R1" s="77"/>
       <c r="S1" s="46"/>
       <c r="T1" s="73" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="U1" s="76"/>
       <c r="V1" s="77"/>
       <c r="W1" s="76" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="X1" s="76"/>
       <c r="Y1" s="77"/>
       <c r="Z1" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AA1" s="78" t="s">
         <v>42</v>
@@ -3097,163 +3314,163 @@
     </row>
     <row r="3" spans="1:29" s="48" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
       <c r="D3" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="F3" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="J3" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="K3" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="L3" s="67" t="s">
+        <v>61</v>
+      </c>
+      <c r="M3" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="N3" s="67" t="s">
         <v>99</v>
       </c>
-      <c r="F3" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="G3" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="H3" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="I3" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="J3" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="K3" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="L3" s="67" t="s">
+      <c r="O3" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="P3" s="67" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q3" s="67" t="s">
         <v>62</v>
       </c>
-      <c r="M3" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="N3" s="67" t="s">
-        <v>100</v>
-      </c>
-      <c r="O3" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="P3" s="67" t="s">
+      <c r="R3" s="67" t="s">
+        <v>99</v>
+      </c>
+      <c r="S3" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="T3" s="67" t="s">
+        <v>61</v>
+      </c>
+      <c r="U3" s="67" t="s">
         <v>62</v>
       </c>
-      <c r="Q3" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="R3" s="67" t="s">
-        <v>100</v>
-      </c>
-      <c r="S3" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="T3" s="67" t="s">
+      <c r="V3" s="47" t="s">
+        <v>99</v>
+      </c>
+      <c r="W3" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="X3" s="67" t="s">
         <v>62</v>
       </c>
-      <c r="U3" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="V3" s="47" t="s">
-        <v>100</v>
-      </c>
-      <c r="W3" s="56" t="s">
+      <c r="Y3" s="47" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z3" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA3" s="67" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB3" s="67" t="s">
         <v>62</v>
       </c>
-      <c r="X3" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y3" s="47" t="s">
-        <v>100</v>
-      </c>
-      <c r="Z3" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA3" s="67" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB3" s="67" t="s">
-        <v>63</v>
-      </c>
       <c r="AC3" s="67" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:29" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C4" s="44"/>
       <c r="D4" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F4" s="49" t="s">
+        <v>132</v>
+      </c>
+      <c r="G4" s="49" t="s">
         <v>133</v>
       </c>
-      <c r="G4" s="49" t="s">
+      <c r="H4" s="49" t="s">
         <v>134</v>
       </c>
-      <c r="H4" s="49" t="s">
+      <c r="I4" s="49" t="s">
         <v>135</v>
       </c>
-      <c r="I4" s="49" t="s">
+      <c r="J4" s="49" t="s">
         <v>136</v>
-      </c>
-      <c r="J4" s="49" t="s">
-        <v>137</v>
       </c>
       <c r="K4" s="50"/>
       <c r="L4" s="51">
         <v>1</v>
       </c>
       <c r="M4" s="53" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N4" s="49" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O4" s="51"/>
       <c r="P4" s="51" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q4" s="51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R4" s="51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="S4" s="51"/>
       <c r="T4" s="51" t="s">
+        <v>124</v>
+      </c>
+      <c r="U4" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="V4" s="49" t="s">
+        <v>129</v>
+      </c>
+      <c r="W4" s="51" t="s">
         <v>125</v>
       </c>
-      <c r="U4" s="8" t="s">
+      <c r="X4" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="V4" s="49" t="s">
+      <c r="Y4" s="49" t="s">
         <v>130</v>
-      </c>
-      <c r="W4" s="51" t="s">
-        <v>126</v>
-      </c>
-      <c r="X4" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y4" s="49" t="s">
-        <v>131</v>
       </c>
       <c r="Z4" s="52"/>
       <c r="AA4" s="51">
         <v>1</v>
       </c>
       <c r="AB4" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AC4" s="49" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:29" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -3343,7 +3560,7 @@
       <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="W5" sqref="W5"/>
+      <selection pane="bottomRight" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3389,50 +3606,50 @@
       <c r="E1" s="81"/>
       <c r="F1" s="18"/>
       <c r="G1" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="J1" s="25" t="s">
         <v>155</v>
-      </c>
-      <c r="H1" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="I1" s="25" t="s">
-        <v>158</v>
-      </c>
-      <c r="J1" s="25" t="s">
-        <v>156</v>
       </c>
       <c r="K1" s="25" t="s">
         <v>27</v>
       </c>
       <c r="L1" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M1" s="78" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N1" s="74"/>
       <c r="O1" s="75"/>
       <c r="P1" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q1" s="73" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R1" s="76"/>
       <c r="S1" s="77"/>
       <c r="T1" s="46"/>
       <c r="U1" s="73" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="V1" s="76"/>
       <c r="W1" s="77"/>
       <c r="X1" s="68"/>
       <c r="Y1" s="73" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Z1" s="76"/>
       <c r="AA1" s="77"/>
       <c r="AB1" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AC1" s="78" t="s">
         <v>42</v>
@@ -3478,10 +3695,10 @@
         <v>18</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D3" s="25" t="s">
         <v>19</v>
@@ -3490,93 +3707,93 @@
         <v>20</v>
       </c>
       <c r="F3" s="70" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G3" s="72" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" s="72" t="s">
         <v>100</v>
       </c>
-      <c r="H3" s="72" t="s">
+      <c r="I3" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="I3" s="72" t="s">
+      <c r="J3" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="J3" s="72" t="s">
+      <c r="K3" s="72" t="s">
         <v>103</v>
       </c>
-      <c r="K3" s="72" t="s">
-        <v>104</v>
-      </c>
       <c r="L3" s="70" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M3" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="N3" s="32" t="s">
-        <v>63</v>
-      </c>
       <c r="O3" s="32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P3" s="70" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q3" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="R3" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="R3" s="32" t="s">
-        <v>63</v>
-      </c>
       <c r="S3" s="32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="T3" s="70" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="U3" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="V3" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="V3" s="32" t="s">
-        <v>63</v>
-      </c>
       <c r="W3" s="32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="X3" s="70" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Y3" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z3" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="Z3" s="32" t="s">
-        <v>63</v>
-      </c>
       <c r="AA3" s="32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AB3" s="70" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AC3" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD3" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="AD3" s="32" t="s">
-        <v>63</v>
-      </c>
       <c r="AE3" s="32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:31" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="54" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="55" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C4" s="49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="49" t="s">
         <v>26</v>
@@ -3586,65 +3803,65 @@
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="I4" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="J4" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="K4" s="8" t="s">
         <v>149</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>150</v>
       </c>
       <c r="L4" s="50"/>
       <c r="M4" s="57" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N4" s="58" t="s">
         <v>33</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q4" s="51" t="s">
+        <v>151</v>
+      </c>
+      <c r="R4" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="S4" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="U4" s="51" t="s">
         <v>152</v>
       </c>
-      <c r="R4" s="57" t="s">
-        <v>107</v>
-      </c>
-      <c r="S4" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="U4" s="51" t="s">
+      <c r="V4" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="W4" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y4" s="51" t="s">
         <v>153</v>
       </c>
-      <c r="V4" s="51" t="s">
+      <c r="Z4" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="W4" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="Y4" s="51" t="s">
-        <v>154</v>
-      </c>
-      <c r="Z4" s="8" t="s">
-        <v>123</v>
-      </c>
       <c r="AA4" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AC4" s="8">
         <v>1</v>
       </c>
       <c r="AD4" s="53" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AE4" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -3726,10 +3943,10 @@
   <sheetData>
     <row r="1" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C1" s="20"/>
     </row>
@@ -3754,7 +3971,9 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3767,7 +3986,7 @@
         <v>37</v>
       </c>
       <c r="B1" s="35">
-        <v>43489</v>
+        <v>43492</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3780,10 +3999,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>88</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout de la mise en évidence des direction qui expirent
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele.xlsx
+++ b/fichiers/conf/modele.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66537B2-F4B6-4ECF-A7E4-18C3839065D5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C896958-6E2E-4BB0-9AD6-090235D77CDD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2055" yWindow="255" windowWidth="26160" windowHeight="13935" tabRatio="477" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="885" yWindow="705" windowWidth="24960" windowHeight="13320" tabRatio="591" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Responsables" sheetId="1" r:id="rId1"/>
@@ -953,9 +953,6 @@
     <t>&lt;jt:if test="${chef.qualif.dirsf.pasok}"&gt;${chef.qualif.dirsf.finvalidite}&lt;/jt:if&gt;</t>
   </si>
   <si>
-    <t>&lt;jt:if test="${chef.qualif.dirsf.ok}"&gt;${chef.qualif.dirsf.finvalidite}&lt;/jt:if&gt;</t>
-  </si>
-  <si>
     <t>${global.groupe}</t>
   </si>
   <si>
@@ -1333,6 +1330,9 @@
   </si>
   <si>
     <t>${chef.formation.accueil_scoutisme_rg.datefin}</t>
+  </si>
+  <si>
+    <t>&lt;jt:if test="${chef.qualif.dirsf.ok}" onProcessed="org.leplan73.outilssgdf.gui.QualifDirSfListener"&gt;${chef.qualif.dirsf.finvalidite}&lt;/jt:if&gt;</t>
   </si>
 </sst>
 </file>
@@ -2519,7 +2519,7 @@
         <v>18</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F1" s="25" t="s">
         <v>68</v>
@@ -2528,55 +2528,55 @@
         <v>54</v>
       </c>
       <c r="H1" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="J1" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="K1" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="L1" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="L1" s="37" t="s">
-        <v>81</v>
-      </c>
       <c r="M1" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="N1" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="N1" s="41" t="s">
-        <v>91</v>
-      </c>
       <c r="O1" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P1" s="27" t="s">
         <v>66</v>
       </c>
       <c r="Q1" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="R1" s="39" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="S1" s="39" t="s">
+        <v>179</v>
+      </c>
+      <c r="T1" s="39" t="s">
         <v>180</v>
       </c>
-      <c r="T1" s="39" t="s">
-        <v>181</v>
-      </c>
       <c r="U1" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="V1" s="39" t="s">
+        <v>189</v>
+      </c>
+      <c r="W1" s="39" t="s">
         <v>186</v>
       </c>
-      <c r="V1" s="39" t="s">
-        <v>190</v>
-      </c>
-      <c r="W1" s="39" t="s">
-        <v>187</v>
-      </c>
       <c r="X1" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="Y1" s="39" t="s">
         <v>9</v>
@@ -2585,19 +2585,19 @@
         <v>10</v>
       </c>
       <c r="AA1" s="39" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AB1" s="39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AC1" s="39" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AD1" s="39" t="s">
+        <v>171</v>
+      </c>
+      <c r="AE1" s="39" t="s">
         <v>172</v>
-      </c>
-      <c r="AE1" s="39" t="s">
-        <v>173</v>
       </c>
       <c r="AF1" s="39" t="s">
         <v>11</v>
@@ -2606,19 +2606,19 @@
         <v>12</v>
       </c>
       <c r="AH1" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI1" s="39" t="s">
+        <v>177</v>
+      </c>
+      <c r="AJ1" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="AK1" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="AI1" s="39" t="s">
-        <v>178</v>
-      </c>
-      <c r="AJ1" s="39" t="s">
-        <v>179</v>
-      </c>
-      <c r="AK1" s="39" t="s">
-        <v>116</v>
-      </c>
       <c r="AL1" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AM1" s="40" t="s">
         <v>13</v>
@@ -2642,21 +2642,21 @@
         <v>17</v>
       </c>
       <c r="AT1" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AU1" s="22" t="s">
         <v>6</v>
       </c>
       <c r="AV1" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AW1" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -2668,7 +2668,7 @@
         <v>56</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F2" s="16" t="s">
         <v>69</v>
@@ -2677,7 +2677,7 @@
         <v>64</v>
       </c>
       <c r="I2" s="38" t="s">
-        <v>72</v>
+        <v>193</v>
       </c>
       <c r="J2" s="38" t="s">
         <v>71</v>
@@ -2689,10 +2689,10 @@
         <v>60</v>
       </c>
       <c r="M2" s="42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N2" s="42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O2" s="10"/>
       <c r="P2" s="10" t="s">
@@ -2700,25 +2700,25 @@
       </c>
       <c r="Q2" s="10"/>
       <c r="R2" s="38" t="s">
+        <v>182</v>
+      </c>
+      <c r="S2" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="S2" s="38" t="s">
+      <c r="T2" s="38" t="s">
         <v>184</v>
       </c>
-      <c r="T2" s="38" t="s">
-        <v>185</v>
-      </c>
       <c r="U2" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="V2" s="38" t="s">
+        <v>190</v>
+      </c>
+      <c r="W2" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="V2" s="38" t="s">
-        <v>191</v>
-      </c>
-      <c r="W2" s="38" t="s">
-        <v>189</v>
-      </c>
       <c r="X2" s="38" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Y2" s="38" t="s">
         <v>44</v>
@@ -2727,19 +2727,19 @@
         <v>45</v>
       </c>
       <c r="AA2" s="38" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AB2" s="38" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AC2" s="38" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AD2" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="AE2" s="38" t="s">
         <v>170</v>
-      </c>
-      <c r="AE2" s="38" t="s">
-        <v>171</v>
       </c>
       <c r="AF2" s="38" t="s">
         <v>46</v>
@@ -2748,16 +2748,16 @@
         <v>47</v>
       </c>
       <c r="AH2" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="AI2" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="AI2" s="38" t="s">
+      <c r="AJ2" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="AJ2" s="38" t="s">
+      <c r="AK2" s="38" t="s">
         <v>119</v>
-      </c>
-      <c r="AK2" s="38" t="s">
-        <v>120</v>
       </c>
       <c r="AL2" s="10"/>
       <c r="AM2" s="38" t="s">
@@ -2779,22 +2779,22 @@
         <v>52</v>
       </c>
       <c r="AS2" s="38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AT2" s="3"/>
       <c r="AU2" s="36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AV2" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AW2" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:49" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>1</v>
@@ -2806,7 +2806,7 @@
         <v>56</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>69</v>
@@ -2815,7 +2815,7 @@
         <v>64</v>
       </c>
       <c r="I3" s="38" t="s">
-        <v>72</v>
+        <v>193</v>
       </c>
       <c r="J3" s="38" t="s">
         <v>71</v>
@@ -2827,10 +2827,10 @@
         <v>60</v>
       </c>
       <c r="M3" s="42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N3" s="42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O3" s="10"/>
       <c r="P3" s="10" t="s">
@@ -2838,25 +2838,25 @@
       </c>
       <c r="Q3" s="10"/>
       <c r="R3" s="38" t="s">
+        <v>182</v>
+      </c>
+      <c r="S3" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="S3" s="38" t="s">
+      <c r="T3" s="38" t="s">
         <v>184</v>
       </c>
-      <c r="T3" s="38" t="s">
-        <v>185</v>
-      </c>
       <c r="U3" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="V3" s="38" t="s">
+        <v>190</v>
+      </c>
+      <c r="W3" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="V3" s="38" t="s">
-        <v>191</v>
-      </c>
-      <c r="W3" s="38" t="s">
-        <v>189</v>
-      </c>
       <c r="X3" s="38" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Y3" s="38" t="s">
         <v>44</v>
@@ -2865,19 +2865,19 @@
         <v>45</v>
       </c>
       <c r="AA3" s="38" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AB3" s="38" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AC3" s="38" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AD3" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="AE3" s="38" t="s">
         <v>170</v>
-      </c>
-      <c r="AE3" s="38" t="s">
-        <v>171</v>
       </c>
       <c r="AF3" s="38" t="s">
         <v>46</v>
@@ -2886,16 +2886,16 @@
         <v>47</v>
       </c>
       <c r="AH3" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="AI3" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="AI3" s="38" t="s">
+      <c r="AJ3" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="AJ3" s="38" t="s">
+      <c r="AK3" s="38" t="s">
         <v>119</v>
-      </c>
-      <c r="AK3" s="38" t="s">
-        <v>120</v>
       </c>
       <c r="AL3" s="10"/>
       <c r="AM3" s="38" t="s">
@@ -2917,17 +2917,17 @@
         <v>52</v>
       </c>
       <c r="AS3" s="38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AT3" s="3"/>
       <c r="AU3" s="36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AV3" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AW3" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -3020,13 +3020,13 @@
         <v>18</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C1" s="22" t="s">
         <v>68</v>
       </c>
       <c r="D1" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E1" s="22" t="s">
         <v>19</v>
@@ -3038,7 +3038,7 @@
         <v>21</v>
       </c>
       <c r="H1" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I1" s="26" t="s">
         <v>23</v>
@@ -3047,7 +3047,7 @@
         <v>22</v>
       </c>
       <c r="K1" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L1" s="39" t="s">
         <v>8</v>
@@ -3059,22 +3059,22 @@
         <v>10</v>
       </c>
       <c r="O1" s="28" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="P1" s="28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Q1" s="39" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="R1" s="39" t="s">
+        <v>171</v>
+      </c>
+      <c r="S1" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="S1" s="39" t="s">
-        <v>173</v>
-      </c>
       <c r="T1" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="U1" s="29" t="s">
         <v>27</v>
@@ -3097,7 +3097,7 @@
         <v>63</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>70</v>
@@ -3130,19 +3130,19 @@
         <v>30</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q2" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="R2" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="R2" s="18" t="s">
+      <c r="S2" s="18" t="s">
         <v>175</v>
-      </c>
-      <c r="S2" s="18" t="s">
-        <v>176</v>
       </c>
       <c r="T2" s="10"/>
       <c r="U2" s="2" t="s">
@@ -3233,49 +3233,49 @@
       <c r="D1" s="45"/>
       <c r="E1" s="45"/>
       <c r="F1" s="25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G1" s="25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H1" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" s="25" t="s">
         <v>112</v>
-      </c>
-      <c r="I1" s="25" t="s">
-        <v>113</v>
       </c>
       <c r="J1" s="25" t="s">
         <v>27</v>
       </c>
       <c r="K1" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L1" s="73" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M1" s="74"/>
       <c r="N1" s="75"/>
       <c r="O1" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P1" s="73" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q1" s="76"/>
       <c r="R1" s="77"/>
       <c r="S1" s="46"/>
       <c r="T1" s="73" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="U1" s="76"/>
       <c r="V1" s="77"/>
       <c r="W1" s="76" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="X1" s="76"/>
       <c r="Y1" s="77"/>
       <c r="Z1" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AA1" s="78" t="s">
         <v>42</v>
@@ -3314,33 +3314,33 @@
     </row>
     <row r="3" spans="1:29" s="48" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
       <c r="D3" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="E3" s="25" t="s">
-        <v>98</v>
-      </c>
       <c r="F3" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G3" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="I3" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="J3" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="J3" s="25" t="s">
-        <v>103</v>
-      </c>
       <c r="K3" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L3" s="67" t="s">
         <v>61</v>
@@ -3349,10 +3349,10 @@
         <v>62</v>
       </c>
       <c r="N3" s="67" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O3" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P3" s="67" t="s">
         <v>61</v>
@@ -3361,10 +3361,10 @@
         <v>62</v>
       </c>
       <c r="R3" s="67" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S3" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="T3" s="67" t="s">
         <v>61</v>
@@ -3373,7 +3373,7 @@
         <v>62</v>
       </c>
       <c r="V3" s="47" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="W3" s="56" t="s">
         <v>61</v>
@@ -3382,10 +3382,10 @@
         <v>62</v>
       </c>
       <c r="Y3" s="47" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z3" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AA3" s="67" t="s">
         <v>61</v>
@@ -3394,12 +3394,12 @@
         <v>62</v>
       </c>
       <c r="AC3" s="67" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:29" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C4" s="44"/>
       <c r="D4" s="8" t="s">
@@ -3409,68 +3409,68 @@
         <v>57</v>
       </c>
       <c r="F4" s="49" t="s">
+        <v>131</v>
+      </c>
+      <c r="G4" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="G4" s="49" t="s">
+      <c r="H4" s="49" t="s">
         <v>133</v>
       </c>
-      <c r="H4" s="49" t="s">
+      <c r="I4" s="49" t="s">
         <v>134</v>
       </c>
-      <c r="I4" s="49" t="s">
+      <c r="J4" s="49" t="s">
         <v>135</v>
-      </c>
-      <c r="J4" s="49" t="s">
-        <v>136</v>
       </c>
       <c r="K4" s="50"/>
       <c r="L4" s="51">
         <v>1</v>
       </c>
       <c r="M4" s="53" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N4" s="49" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O4" s="51"/>
       <c r="P4" s="51" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Q4" s="51" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="R4" s="51" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="S4" s="51"/>
       <c r="T4" s="51" t="s">
+        <v>123</v>
+      </c>
+      <c r="U4" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="V4" s="49" t="s">
+        <v>128</v>
+      </c>
+      <c r="W4" s="51" t="s">
         <v>124</v>
       </c>
-      <c r="U4" s="8" t="s">
+      <c r="X4" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="V4" s="49" t="s">
+      <c r="Y4" s="49" t="s">
         <v>129</v>
-      </c>
-      <c r="W4" s="51" t="s">
-        <v>125</v>
-      </c>
-      <c r="X4" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="Y4" s="49" t="s">
-        <v>130</v>
       </c>
       <c r="Z4" s="52"/>
       <c r="AA4" s="51">
         <v>1</v>
       </c>
       <c r="AB4" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AC4" s="49" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:29" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -3606,22 +3606,22 @@
       <c r="E1" s="81"/>
       <c r="F1" s="18"/>
       <c r="G1" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="J1" s="25" t="s">
         <v>154</v>
-      </c>
-      <c r="H1" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="I1" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="J1" s="25" t="s">
-        <v>155</v>
       </c>
       <c r="K1" s="25" t="s">
         <v>27</v>
       </c>
       <c r="L1" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M1" s="78" t="s">
         <v>58</v>
@@ -3629,27 +3629,27 @@
       <c r="N1" s="74"/>
       <c r="O1" s="75"/>
       <c r="P1" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q1" s="73" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="R1" s="76"/>
       <c r="S1" s="77"/>
       <c r="T1" s="46"/>
       <c r="U1" s="73" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="V1" s="76"/>
       <c r="W1" s="77"/>
       <c r="X1" s="68"/>
       <c r="Y1" s="73" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="Z1" s="76"/>
       <c r="AA1" s="77"/>
       <c r="AB1" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AC1" s="78" t="s">
         <v>42</v>
@@ -3695,7 +3695,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>68</v>
@@ -3707,25 +3707,25 @@
         <v>20</v>
       </c>
       <c r="F3" s="70" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G3" s="72" t="s">
+        <v>98</v>
+      </c>
+      <c r="H3" s="72" t="s">
         <v>99</v>
       </c>
-      <c r="H3" s="72" t="s">
+      <c r="I3" s="72" t="s">
         <v>100</v>
       </c>
-      <c r="I3" s="72" t="s">
+      <c r="J3" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="J3" s="72" t="s">
+      <c r="K3" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="K3" s="72" t="s">
-        <v>103</v>
-      </c>
       <c r="L3" s="70" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M3" s="32" t="s">
         <v>61</v>
@@ -3734,10 +3734,10 @@
         <v>62</v>
       </c>
       <c r="O3" s="32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="P3" s="70" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q3" s="32" t="s">
         <v>61</v>
@@ -3746,10 +3746,10 @@
         <v>62</v>
       </c>
       <c r="S3" s="32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="T3" s="70" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="U3" s="32" t="s">
         <v>61</v>
@@ -3758,10 +3758,10 @@
         <v>62</v>
       </c>
       <c r="W3" s="32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="X3" s="70" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Y3" s="32" t="s">
         <v>61</v>
@@ -3770,10 +3770,10 @@
         <v>62</v>
       </c>
       <c r="AA3" s="32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AB3" s="70" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AC3" s="32" t="s">
         <v>61</v>
@@ -3782,7 +3782,7 @@
         <v>62</v>
       </c>
       <c r="AE3" s="32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:31" s="54" customFormat="1" x14ac:dyDescent="0.25">
@@ -3790,7 +3790,7 @@
         <v>63</v>
       </c>
       <c r="B4" s="55" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" s="49" t="s">
         <v>70</v>
@@ -3803,65 +3803,65 @@
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="I4" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="J4" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="K4" s="8" t="s">
         <v>148</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>149</v>
       </c>
       <c r="L4" s="50"/>
       <c r="M4" s="57" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N4" s="58" t="s">
         <v>33</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q4" s="51" t="s">
+        <v>150</v>
+      </c>
+      <c r="R4" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="S4" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="U4" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="R4" s="57" t="s">
-        <v>106</v>
-      </c>
-      <c r="S4" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="U4" s="51" t="s">
+      <c r="V4" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="W4" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y4" s="51" t="s">
         <v>152</v>
       </c>
-      <c r="V4" s="51" t="s">
+      <c r="Z4" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="W4" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="Y4" s="51" t="s">
-        <v>153</v>
-      </c>
-      <c r="Z4" s="8" t="s">
-        <v>122</v>
-      </c>
       <c r="AA4" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AC4" s="8">
         <v>1</v>
       </c>
       <c r="AD4" s="53" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AE4" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -3943,10 +3943,10 @@
   <sheetData>
     <row r="1" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C1" s="20"/>
     </row>
@@ -3971,9 +3971,7 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3986,7 +3984,7 @@
         <v>37</v>
       </c>
       <c r="B1" s="35">
-        <v>43492</v>
+        <v>43502</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3999,10 +3997,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>87</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Affichage des directions qui ont expirés
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele.xlsx
+++ b/fichiers/conf/modele.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C896958-6E2E-4BB0-9AD6-090235D77CDD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB3E8D8-0BF1-4EFC-AAB7-9299E1CA0AA7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="885" yWindow="705" windowWidth="24960" windowHeight="13320" tabRatio="591" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
@@ -1332,7 +1332,7 @@
     <t>${chef.formation.accueil_scoutisme_rg.datefin}</t>
   </si>
   <si>
-    <t>&lt;jt:if test="${chef.qualif.dirsf.ok}" onProcessed="org.leplan73.outilssgdf.gui.QualifDirSfListener"&gt;${chef.qualif.dirsf.finvalidite}&lt;/jt:if&gt;</t>
+    <t>&lt;jt:if test="${chef.qualif.dirsf.aetaetetitulaire}" onProcessed="org.leplan73.outilssgdf.gui.QualifDirSfListener"&gt;${chef.qualif.dirsf.finvalidite}&lt;/jt:if&gt;</t>
   </si>
 </sst>
 </file>

</xml_diff>